<commit_message>
add the test cases 21-60 for limit module
</commit_message>
<xml_diff>
--- a/limits.xlsx
+++ b/limits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed.El-Sawy\Documents\hdb_test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C19A8A-D091-4AB6-B7F0-4C9E0EF7F9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD3F4BB-D917-4FAD-92BA-5883A82C0D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3D412268-5103-411D-BBE4-3652EEC1385B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1665" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="1089">
   <si>
     <t>Limit</t>
   </si>
@@ -5575,6 +5575,1062 @@
     <t>1. Maker logged in 
 2. Limit selected 
 3. Limit cancelled successfully</t>
+  </si>
+  <si>
+    <t>LIM-21</t>
+  </si>
+  <si>
+    <t>limit_cancel_unapproved_credit_limit_maker</t>
+  </si>
+  <si>
+    <t>Cancel a credit limit request that has not yet been approved</t>
+  </si>
+  <si>
+    <t>Unapproved credit limit must exist</t>
+  </si>
+  <si>
+    <t>LIMIT.CANCEL</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.CANCEL 
+3. Search for the unapproved credit limit 
+4. Select and cancel the record</t>
+  </si>
+  <si>
+    <t>Limit Status: Unapproved</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.CANCEL screen opened 
+3. Unapproved limit retrieved 
+4. Limit cancelled successfully</t>
+  </si>
+  <si>
+    <t>Cancellation executed for unapproved limit</t>
+  </si>
+  <si>
+    <t>LIM-22</t>
+  </si>
+  <si>
+    <t>limit_date_field_relationship_validation_on_modify_cancel_maker</t>
+  </si>
+  <si>
+    <t>Validate logical relationships between date fields on Modify/Cancel screen</t>
+  </si>
+  <si>
+    <t>Existing credit limit</t>
+  </si>
+  <si>
+    <t>LIMIT.MODIFY</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.MODIFY 
+3. Input dates in related fields (submission, approval, expiry, review, etc.) 
+4. Validate behavior</t>
+  </si>
+  <si>
+    <t>Dates: Various valid/invalid combinations</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.MODIFY screen opened 
+3. Dates entered 
+4. System enforces logical relationships, error displayed if violated</t>
+  </si>
+  <si>
+    <t>Date logic enforced correctly</t>
+  </si>
+  <si>
+    <t>LIM-23</t>
+  </si>
+  <si>
+    <t>limit_date_field_relationship_validation_on_create_with_collateral_maker</t>
+  </si>
+  <si>
+    <t>Validate logical relationships between date fields during creation of secured limit</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.MAINTENANCE 
+3. Choose secured limit type 
+4. Enter related dates 
+5. Submit</t>
+  </si>
+  <si>
+    <t>Limit Type: Secured; Dates: Various combinations</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.MAINTENANCE screen opened 
+3. Secured type selected 
+4. Dates validated 
+5. Record submitted only if valid</t>
+  </si>
+  <si>
+    <t>Logical date checks enforced</t>
+  </si>
+  <si>
+    <t>LIM-24</t>
+  </si>
+  <si>
+    <t>limit_date_field_relationship_validation_on_create_without_collateral_maker</t>
+  </si>
+  <si>
+    <t>Validate logical date relationships during unsecured limit creation</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.MAINTENANCE 
+3. Choose unsecured limit type 
+4. Enter required dates 
+5. Submit</t>
+  </si>
+  <si>
+    <t>Limit Type: Unsecured; Dates: Various combinations</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.MAINTENANCE screen opened 
+3. Unsecured type selected 
+4. Dates validated 
+5. Record submitted only if valid</t>
+  </si>
+  <si>
+    <t>Date relationships enforced correctly</t>
+  </si>
+  <si>
+    <t>LIM-25</t>
+  </si>
+  <si>
+    <t>limit_check_historical_data_fields_on_all_screens_maker</t>
+  </si>
+  <si>
+    <t>Verify historical data fields are displayed correctly across all limit screens</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.INQUIRY 
+3. View history section on multiple screens</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.INQUIRY screen accessed 
+3. Historical data (limits, collateral) displayed with Arabic labels</t>
+  </si>
+  <si>
+    <t>All history fields visible and properly translated</t>
+  </si>
+  <si>
+    <t>LIM-26</t>
+  </si>
+  <si>
+    <t>limit_fields_to_be_removed_from_modify_cancel_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify that specified fields are removed from Modify/Cancel screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.MODIFY 
+3. Check if removed fields (e.g. announced amount) are not displayed</t>
+  </si>
+  <si>
+    <t>Field: Announced Amount</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.MODIFY screen opened 
+3. Specified fields are not visible</t>
+  </si>
+  <si>
+    <t>Unwanted fields successfully removed</t>
+  </si>
+  <si>
+    <t>LIM-27</t>
+  </si>
+  <si>
+    <t>limit_fields_to_be_removed_from_secured_limit_creation_screen_maker</t>
+  </si>
+  <si>
+    <t>Ensure specified fields are removed from secured limit creation screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Select secured limit creation 
+3. Check field list</t>
+  </si>
+  <si>
+    <t>Fields: Announced Amount, Max Amount, Expiry Extension, Country Concentration, etc.</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.MAINTENANCE screen opened 
+3. Specified fields are not shown</t>
+  </si>
+  <si>
+    <t>Fields removed as per requirement</t>
+  </si>
+  <si>
+    <t>LIM-28</t>
+  </si>
+  <si>
+    <t>limit_fields_to_be_removed_from_unsecured_limit_creation_screen_maker</t>
+  </si>
+  <si>
+    <t>Ensure specified fields are removed from unsecured limit creation screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Select unsecured limit creation 
+3. Verify absence of specific fields</t>
+  </si>
+  <si>
+    <t>Fields: Announced Amount, Credit Balance Deduction, Max Amount, etc.</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.MAINTENANCE screen opened 
+3. Specified fields are not visible</t>
+  </si>
+  <si>
+    <t>Fields removed as per specification</t>
+  </si>
+  <si>
+    <t>LIM-29</t>
+  </si>
+  <si>
+    <t>limit_renamed_fields_on_unsecured_limit_screen_maker</t>
+  </si>
+  <si>
+    <t>Check renamed fields on unsecured limit screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to unsecured limit screen 
+3. Verify field labels</t>
+  </si>
+  <si>
+    <t>Old Field Names: Approval Date, Expiry Date, Availability Date, etc.</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.MAINTENANCE screen opened 
+3. Field names shown as per new labels</t>
+  </si>
+  <si>
+    <t>Field labels updated correctly</t>
+  </si>
+  <si>
+    <t>LIM-30</t>
+  </si>
+  <si>
+    <t>limit_renamed_fields_on_secured_limit_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify renamed field labels on secured limit creation screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to secured limit screen 
+3. Check label updates</t>
+  </si>
+  <si>
+    <t>Old Field Names: Approval Date, Expiry Date, Fixed/Variable, etc.</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.MAINTENANCE screen opened 
+3. Field labels updated to new values</t>
+  </si>
+  <si>
+    <t>Field renaming verified</t>
+  </si>
+  <si>
+    <t>limit_rename_fields_input_with_collateral_screen_maker</t>
+  </si>
+  <si>
+    <t>Rename field labels in collateral limit input screen</t>
+  </si>
+  <si>
+    <t>LIMIT.INPUT</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.INPUT screen (with collateral) 
+3. Verify renamed labels</t>
+  </si>
+  <si>
+    <t>Field Names: Approval Date 
+Condition Fulfillment Date, Expiry Date 
+Limit Expiry, Available Date 
+Activation Date, Fixed/Variable 
+Fixed or Variable, Allowed Limits 
+Limit Type</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.INPUT screen accessed 
+3. Field labels updated as specified</t>
+  </si>
+  <si>
+    <t>All field labels reflect new naming convention</t>
+  </si>
+  <si>
+    <t>LIM-31</t>
+  </si>
+  <si>
+    <t>limit_add_fields_amend_cancel_screen_maker</t>
+  </si>
+  <si>
+    <t>Add new fields to amend/cancel screen</t>
+  </si>
+  <si>
+    <t>LIMIT.AMEND</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.AMEND 
+3. Check for new fields: Expiry Extension Date, Credit Authority, First Grant Date</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.AMEND screen accessed 
+3. New fields are displayed</t>
+  </si>
+  <si>
+    <t>All new fields appear correctly on screen</t>
+  </si>
+  <si>
+    <t>LIM-32</t>
+  </si>
+  <si>
+    <t>limit_add_fields_input_with_collateral_screen_maker</t>
+  </si>
+  <si>
+    <t>Add new fields to input screen with collateral</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.INPUT 
+3. Check for new fields: Credit Authority, First Grant Date</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.INPUT screen accessed 
+3. New fields displayed correctly</t>
+  </si>
+  <si>
+    <t>All additional fields are present</t>
+  </si>
+  <si>
+    <t>LIM-33</t>
+  </si>
+  <si>
+    <t>limit_add_fields_input_without_collateral_screen_maker</t>
+  </si>
+  <si>
+    <t>Add new fields to unsecured input screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.INPUT 
+3. Confirm new fields added: Credit Authority, First Grant Date</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.INPUT screen accessed 
+3. Required fields displayed</t>
+  </si>
+  <si>
+    <t>New fields added and visible</t>
+  </si>
+  <si>
+    <t>LIM-34</t>
+  </si>
+  <si>
+    <t>limit_editable_fields_amend_cancel_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify all editable fields in amend/cancel screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.AMEND 
+3. Attempt to edit listed fields</t>
+  </si>
+  <si>
+    <t>Editable fields include: Currency, Concentration, Submission/Approval/Review/Expiry Dates, etc.</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.AMEND screen accessed 
+3. All fields allow editing as expected</t>
+  </si>
+  <si>
+    <t>Editable fields respond correctly</t>
+  </si>
+  <si>
+    <t>LIM-35</t>
+  </si>
+  <si>
+    <t>limit_editable_fields_facility_link_input_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify editable fields in linking credit limit to facility</t>
+  </si>
+  <si>
+    <t>LIMIT.LINK.FACILITY</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.LINK.FACILITY 
+3. Edit credit limit field</t>
+  </si>
+  <si>
+    <t>Limit Field</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Screen accessed 
+3. Field edited successfully</t>
+  </si>
+  <si>
+    <t>Field is editable</t>
+  </si>
+  <si>
+    <t>LIM-36</t>
+  </si>
+  <si>
+    <t>limit_editable_fields_input_with_collateral_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify editable fields in collateral credit limit input</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.INPUT (collateral) 
+3. Edit listed fields</t>
+  </si>
+  <si>
+    <t>Fields include: Currency, Expiry, Concentration, Review Cycle, Activation Date, Guarantee Type, etc.</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.INPUT screen accessed 
+3. All specified fields editable</t>
+  </si>
+  <si>
+    <t>All editable fields are correctly enabled</t>
+  </si>
+  <si>
+    <t>LIM-37</t>
+  </si>
+  <si>
+    <t>limit_editable_fields_input_without_collateral_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify editable fields in unsecured credit limit input</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.INPUT (non-collateral) 
+3. Edit listed fields</t>
+  </si>
+  <si>
+    <t>Fields include: Currency, Expiry, Review Cycle, Activation Date, Credit Authority, Allowed Branches, etc.</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.INPUT screen accessed 
+3. Fields editable</t>
+  </si>
+  <si>
+    <t>Fields function as editable</t>
+  </si>
+  <si>
+    <t>LIM-38</t>
+  </si>
+  <si>
+    <t>limit_non_editable_fields_amend_cancel_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify fields that should be locked in amend/cancel screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.AMEND 
+3. Try editing locked fields</t>
+  </si>
+  <si>
+    <t>Fields: Limit ID, Currency</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Screen opened 
+3. System blocked field edit</t>
+  </si>
+  <si>
+    <t>Non-editable fields remain locked</t>
+  </si>
+  <si>
+    <t>LIM-39</t>
+  </si>
+  <si>
+    <t>limit_non_editable_fields_input_without_collateral_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify locked fields in unsecured credit input</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.INPUT (non-collateral) 
+3. Try editing system-generated ID</t>
+  </si>
+  <si>
+    <t>Field: Credit Limit ID</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.INPUT screen accessed 
+3. Edit blocked</t>
+  </si>
+  <si>
+    <t>Field is locked</t>
+  </si>
+  <si>
+    <t>LIM-40</t>
+  </si>
+  <si>
+    <t>limit_non_editable_fields_facility_link_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify fields that must remain locked in facility linking screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.LINK.FACILITY 
+3. Try editing restricted fields</t>
+  </si>
+  <si>
+    <t>Fields: Account Number, Customer ID, Currency, Account Type, Account Name, Short Name</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Screen opened 
+3. All listed fields are non-editable</t>
+  </si>
+  <si>
+    <t>All fields correctly protected</t>
+  </si>
+  <si>
+    <t>LIM-41</t>
+  </si>
+  <si>
+    <t>limit_non_editable_fields_input_with_collateral_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify locked fields in collateral credit input</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to LIMIT.INPUT (collateral) 
+3. Try editing system fields</t>
+  </si>
+  <si>
+    <t>Fields: Limit ID, Real-time Collateral Value</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. LIMIT.INPUT accessed 
+3. Fields are locked</t>
+  </si>
+  <si>
+    <t>Fields remain non-editable</t>
+  </si>
+  <si>
+    <t>LIM-42</t>
+  </si>
+  <si>
+    <t>limit_auto_description_fields_facility_link_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify automatic description fields in facility link screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Select linked account 
+3. Verify description fields populate automatically</t>
+  </si>
+  <si>
+    <t>Auto fields: Customer ID, Currency, Account Name, Account Type, Short Name</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Selection made 
+3. Fields populated automatically</t>
+  </si>
+  <si>
+    <t>Auto-populated data works as intended</t>
+  </si>
+  <si>
+    <t>LIM-43</t>
+  </si>
+  <si>
+    <t>limit_auto_description_fields_input_with_collateral_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify auto-filled fields in collateral limit input</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Select limit ID and code 
+3. Verify auto-fill fields</t>
+  </si>
+  <si>
+    <t>Auto fields: Limit Name, Currency, Guarantee, Submission/Approval Dates, etc.</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Selection made 
+3. Descriptions auto-filled</t>
+  </si>
+  <si>
+    <t>System auto-fills descriptions correctly</t>
+  </si>
+  <si>
+    <t>LIM-44</t>
+  </si>
+  <si>
+    <t>limit_auto_description_fields_amend_cancel_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify auto-filled fields in amend/cancel screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Select limit record 
+3. Review auto-filled fields</t>
+  </si>
+  <si>
+    <t>Auto fields: Limit Name, Guarantee, Dates, Credit Authority</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Record selected 
+3. Fields display expected values</t>
+  </si>
+  <si>
+    <t>All auto-filled fields populated</t>
+  </si>
+  <si>
+    <t>LIM-45</t>
+  </si>
+  <si>
+    <t>limit_auto_description_fields_input_without_collateral_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify auto-filled fields in unsecured input screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Select unsecured limit ID 
+3. Check descriptions</t>
+  </si>
+  <si>
+    <t>Fields: Limit Name, Currency, Review Date, Expiry, Guarantee</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Record selected 
+3. Descriptions shown</t>
+  </si>
+  <si>
+    <t>Auto-population successful</t>
+  </si>
+  <si>
+    <t>LIM-46</t>
+  </si>
+  <si>
+    <t>limit_default_guarantee_field_amend_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify default display of "Real-time Guarantee Update" field</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to amend screen 
+3. Check default value for field</t>
+  </si>
+  <si>
+    <t>Field: Real-time Guarantee Update</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Field shown with value YES</t>
+  </si>
+  <si>
+    <t>Default value appears correctly</t>
+  </si>
+  <si>
+    <t>LIM-47</t>
+  </si>
+  <si>
+    <t>limit_mandatory_fields_amend_cancel_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify mandatory fields in amend/cancel screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to screen 
+3. Leave mandatory fields empty 
+4. Attempt to submit</t>
+  </si>
+  <si>
+    <t>Fields: Credit Authority, First Grant Date</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Mandatory fields left blank 
+3. Submission blocked</t>
+  </si>
+  <si>
+    <t>System enforces required field entry</t>
+  </si>
+  <si>
+    <t>LIM-48</t>
+  </si>
+  <si>
+    <t>limit_mandatory_fields_facility_link_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify mandatory fields in credit limit to facility screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Leave credit limit ID blank 
+3. Try to proceed</t>
+  </si>
+  <si>
+    <t>Field: Limit ID</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Required field left blank 
+3. Submission blocked</t>
+  </si>
+  <si>
+    <t>System blocks empty required fields</t>
+  </si>
+  <si>
+    <t>LIM-49</t>
+  </si>
+  <si>
+    <t>limit_mandatory_fields_input_with_collateral_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify mandatory fields in collateral credit input screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Navigate to screen 
+3. Leave required fields empty 
+4. Try to submit</t>
+  </si>
+  <si>
+    <t>Required Fields: Limit ID, Approval Date, Currency, Expiry, Review Cycle, Authorized Amount, etc.</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Fields left empty 
+3. Submission failed</t>
+  </si>
+  <si>
+    <t>Submission prevented until all fields filled</t>
+  </si>
+  <si>
+    <t>LIM-50</t>
+  </si>
+  <si>
+    <t>limit_mandatory_fields_input_without_collateral_screen_maker</t>
+  </si>
+  <si>
+    <t>Verify mandatory fields in unsecured input screen</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Leave key fields empty 
+3. Attempt submission</t>
+  </si>
+  <si>
+    <t>Required Fields: Limit ID, Approval Date, Currency, Expiry, Review Cycle, Authorized Amount, Activation Date, etc.</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Fields left blank 
+3. System prevented submission</t>
+  </si>
+  <si>
+    <t>System enforces input requirements</t>
+  </si>
+  <si>
+    <t>LIM-51</t>
+  </si>
+  <si>
+    <t>limit_validate_linking_rules_by_limit_type_maker</t>
+  </si>
+  <si>
+    <t>Verify account linking rules per limit type</t>
+  </si>
+  <si>
+    <t>LIMIT.LINK</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Select different limit types 
+3. Link to accounts</t>
+  </si>
+  <si>
+    <t>Limit Types: Machine Limit, Mortgage, Installment Loan, Operation Limit</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Link screen accessed 
+3. Each type linked as per rule</t>
+  </si>
+  <si>
+    <t>Limit type links respected</t>
+  </si>
+  <si>
+    <t>LIM-52</t>
+  </si>
+  <si>
+    <t>limit_search_cancelled_limits_maker</t>
+  </si>
+  <si>
+    <t>Search for cancelled credit limits</t>
+  </si>
+  <si>
+    <t>LIMIT.SEARCH</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Use various search criteria 
+3. Locate cancelled limits</t>
+  </si>
+  <si>
+    <t>Search by: Customer ID, Customer Name, Limit ID</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Cancelled limits found using criteria</t>
+  </si>
+  <si>
+    <t>Search returns valid results</t>
+  </si>
+  <si>
+    <t>LIM-53</t>
+  </si>
+  <si>
+    <t>limit_auto_sequence_validation_input_with_collateral_maker</t>
+  </si>
+  <si>
+    <t>Verify auto-numbering sequence for multiple limits with collateral</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Create multiple limits for same customer/product 
+3. Check serials</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Serial auto-incremented correctly</t>
+  </si>
+  <si>
+    <t>Auto-sequence assigned properly</t>
+  </si>
+  <si>
+    <t>LIM-54</t>
+  </si>
+  <si>
+    <t>limit_auto_sequence_validation_input_without_collateral_maker</t>
+  </si>
+  <si>
+    <t>Verify auto-numbering sequence for multiple limits without collateral</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Create multiple unsecured limits 
+3. Check limit IDs</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. IDs auto-increment as expected</t>
+  </si>
+  <si>
+    <t>Serials assigned automatically</t>
+  </si>
+  <si>
+    <t>LIM-55</t>
+  </si>
+  <si>
+    <t>limit_check_credit_authority_table_maker</t>
+  </si>
+  <si>
+    <t>Validate content of CREDIT.AUTHORITY table</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>CREDIT.AUTHORITY</t>
+  </si>
+  <si>
+    <t>1. Login to DB 
+2. Query CREDIT.AUTHORITY table 
+3. Check for valid entries</t>
+  </si>
+  <si>
+    <t>1. Table contains values per BRD</t>
+  </si>
+  <si>
+    <t>Data matches specification</t>
+  </si>
+  <si>
+    <t>LIM-56</t>
+  </si>
+  <si>
+    <t>limit_check_cancelled_limit_report_maker</t>
+  </si>
+  <si>
+    <t>Validate fields in cancelled limit report</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>LIMIT.REPORT</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Generate cancelled limits report 
+3. Check report structure</t>
+  </si>
+  <si>
+    <t>Fields: Limit ID, Currency, Approval Date, Review Cycle, Expiry, Authorized, Covered, Uncovered Amount</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Report includes all fields 
+3. Data consistent</t>
+  </si>
+  <si>
+    <t>Report structure and content correct</t>
+  </si>
+  <si>
+    <t>LIM-57</t>
+  </si>
+  <si>
+    <t>limit_uncovered_amount_field_validation_maker</t>
+  </si>
+  <si>
+    <t>Test uncovered amount logic with partial collateral</t>
+  </si>
+  <si>
+    <t>1. Create limit for 100k 
+2. Collateral 80k 
+3. Fill uncovered field as 20k 
+4. Use limit</t>
+  </si>
+  <si>
+    <t>Limit: 100000; Collateral: 80000; Uncovered: 20000</t>
+  </si>
+  <si>
+    <t>1. Maker created limit 
+2. System allowed usage without errors</t>
+  </si>
+  <si>
+    <t>System handles uncovered logic correctly</t>
+  </si>
+  <si>
+    <t>LIM-58</t>
+  </si>
+  <si>
+    <t>limit_edit_during_creation_before_execution_maker</t>
+  </si>
+  <si>
+    <t>Edit limit values before execution</t>
+  </si>
+  <si>
+    <t>1. Enter all fields 
+2. Submit 
+3. Modify amount from 100k to 200k 
+4. Submit</t>
+  </si>
+  <si>
+    <t>Amount: 100000 → 200000</t>
+  </si>
+  <si>
+    <t>1. Maker edits before execution 
+2. Submission accepted</t>
+  </si>
+  <si>
+    <t>System allows edits before execution</t>
+  </si>
+  <si>
+    <t>LIM-59</t>
+  </si>
+  <si>
+    <t>limit_post_usage_field_auto_update_maker</t>
+  </si>
+  <si>
+    <t>Verify automatic field update after limit usage</t>
+  </si>
+  <si>
+    <t>Limit must be created and used</t>
+  </si>
+  <si>
+    <t>1. Use limit partially 
+2. Review auto-filled fields</t>
+  </si>
+  <si>
+    <t>Fields: Used Amount, Available Amount, Guarantee No., Limit ID, Limit Type</t>
+  </si>
+  <si>
+    <t>1. Fields updated as per usage</t>
+  </si>
+  <si>
+    <t>Fields update automatically after usage</t>
+  </si>
+  <si>
+    <t>LIM-60</t>
+  </si>
+  <si>
+    <t>limit_search_existing_limit_inquiry_maker</t>
+  </si>
+  <si>
+    <t>Verify inquiry screen displays all expected data</t>
+  </si>
+  <si>
+    <t>Limit must be created</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+2. Search by limit ID 
+3. Confirm field values</t>
+  </si>
+  <si>
+    <t>Limit ID: LIM01234</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+2. Fields populated 
+3. Values match what was entered</t>
+  </si>
+  <si>
+    <t>Inquiry screen data is consistent</t>
   </si>
 </sst>
 </file>
@@ -5643,7 +6699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -5661,6 +6717,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -10585,9 +11644,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB919F80-9B96-4E34-ADD6-E7884B62F830}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -10605,9 +11664,9 @@
     <col min="10" max="10" width="19" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.21875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="51.77734375" style="6"/>
+    <col min="13" max="13" width="50.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="49" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="51.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="51.21875" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="46" style="6" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="51.77734375" style="6"/>
@@ -10666,7 +11725,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -10719,7 +11778,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -10772,7 +11831,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -10825,7 +11884,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -10878,7 +11937,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -10931,7 +11990,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -10984,7 +12043,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -11037,7 +12096,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -11090,7 +12149,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -11143,7 +12202,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -11196,7 +12255,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -11249,7 +12308,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -11302,7 +12361,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -11355,7 +12414,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -11408,7 +12467,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -11461,7 +12520,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -11567,7 +12626,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -11673,7 +12732,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -11723,6 +12782,2179 @@
         <v>754</v>
       </c>
       <c r="Q21" s="4" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>795</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>796</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>797</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>798</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H22" s="6">
+        <v>1</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>799</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L22" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>800</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>801</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>802</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>803</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>804</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>805</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>806</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>807</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H23" s="6">
+        <v>1</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>808</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L23" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>809</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>811</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>812</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>813</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>814</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>815</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H24" s="6">
+        <v>1</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>816</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>817</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="72" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>820</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>821</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H25" s="6">
+        <v>1</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="Q25" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>828</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H26" s="6">
+        <v>1</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L26" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>831</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="Q26" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>835</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H27" s="6">
+        <v>1</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>808</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>836</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>837</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>838</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>839</v>
+      </c>
+      <c r="Q27" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>840</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>841</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>842</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H28" s="6">
+        <v>1</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L28" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>843</v>
+      </c>
+      <c r="N28" s="6" t="s">
+        <v>844</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>845</v>
+      </c>
+      <c r="P28" s="6" t="s">
+        <v>846</v>
+      </c>
+      <c r="Q28" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>847</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>848</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>849</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H29" s="6">
+        <v>1</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L29" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>850</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>851</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>852</v>
+      </c>
+      <c r="P29" s="6" t="s">
+        <v>853</v>
+      </c>
+      <c r="Q29" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>854</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>855</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>856</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H30" s="6">
+        <v>1</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L30" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>857</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>858</v>
+      </c>
+      <c r="O30" s="6" t="s">
+        <v>859</v>
+      </c>
+      <c r="P30" s="6" t="s">
+        <v>860</v>
+      </c>
+      <c r="Q30" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>861</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>862</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>863</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H31" s="6">
+        <v>1</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L31" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>864</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>865</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>866</v>
+      </c>
+      <c r="P31" s="6" t="s">
+        <v>867</v>
+      </c>
+      <c r="Q31" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="6">
+        <v>30</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>861</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>868</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>869</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H32" s="6">
+        <v>1</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L32" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>871</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>872</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>873</v>
+      </c>
+      <c r="P32" s="6" t="s">
+        <v>874</v>
+      </c>
+      <c r="Q32" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="6">
+        <v>31</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>875</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>876</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>877</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H33" s="6">
+        <v>1</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L33" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>879</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>880</v>
+      </c>
+      <c r="P33" s="6" t="s">
+        <v>881</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="6">
+        <v>32</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>882</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>883</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>884</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H34" s="6">
+        <v>1</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L34" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>885</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="O34" s="6" t="s">
+        <v>886</v>
+      </c>
+      <c r="P34" s="6" t="s">
+        <v>887</v>
+      </c>
+      <c r="Q34" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="6">
+        <v>33</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>888</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>889</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>890</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H35" s="6">
+        <v>1</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L35" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>891</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>892</v>
+      </c>
+      <c r="P35" s="6" t="s">
+        <v>893</v>
+      </c>
+      <c r="Q35" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="6">
+        <v>34</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>894</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>895</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>896</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H36" s="6">
+        <v>1</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L36" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>897</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>898</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>899</v>
+      </c>
+      <c r="P36" s="6" t="s">
+        <v>900</v>
+      </c>
+      <c r="Q36" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="6">
+        <v>35</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>901</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>902</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>903</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H37" s="6">
+        <v>1</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>904</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L37" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>905</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>906</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>907</v>
+      </c>
+      <c r="P37" s="6" t="s">
+        <v>908</v>
+      </c>
+      <c r="Q37" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="6">
+        <v>36</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>909</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>910</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>911</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H38" s="6">
+        <v>1</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L38" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M38" s="6" t="s">
+        <v>912</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>913</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>914</v>
+      </c>
+      <c r="P38" s="6" t="s">
+        <v>915</v>
+      </c>
+      <c r="Q38" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="6">
+        <v>37</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>916</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>917</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>918</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H39" s="6">
+        <v>1</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L39" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>919</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>920</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>921</v>
+      </c>
+      <c r="P39" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="Q39" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
+        <v>38</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>923</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>924</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>925</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H40" s="6">
+        <v>1</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L40" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M40" s="6" t="s">
+        <v>926</v>
+      </c>
+      <c r="N40" s="6" t="s">
+        <v>927</v>
+      </c>
+      <c r="O40" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="P40" s="6" t="s">
+        <v>929</v>
+      </c>
+      <c r="Q40" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="6">
+        <v>39</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>930</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>931</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>932</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H41" s="6">
+        <v>1</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L41" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>933</v>
+      </c>
+      <c r="N41" s="6" t="s">
+        <v>934</v>
+      </c>
+      <c r="O41" s="6" t="s">
+        <v>935</v>
+      </c>
+      <c r="P41" s="6" t="s">
+        <v>936</v>
+      </c>
+      <c r="Q41" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
+        <v>40</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>937</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>938</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>939</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H42" s="6">
+        <v>1</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>904</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L42" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M42" s="6" t="s">
+        <v>940</v>
+      </c>
+      <c r="N42" s="6" t="s">
+        <v>941</v>
+      </c>
+      <c r="O42" s="6" t="s">
+        <v>942</v>
+      </c>
+      <c r="P42" s="6" t="s">
+        <v>943</v>
+      </c>
+      <c r="Q42" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="6">
+        <v>41</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>944</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>945</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>946</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H43" s="6">
+        <v>1</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L43" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>947</v>
+      </c>
+      <c r="N43" s="6" t="s">
+        <v>948</v>
+      </c>
+      <c r="O43" s="6" t="s">
+        <v>949</v>
+      </c>
+      <c r="P43" s="6" t="s">
+        <v>950</v>
+      </c>
+      <c r="Q43" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="6">
+        <v>42</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>951</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H44" s="6">
+        <v>1</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>904</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L44" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M44" s="6" t="s">
+        <v>954</v>
+      </c>
+      <c r="N44" s="6" t="s">
+        <v>955</v>
+      </c>
+      <c r="O44" s="6" t="s">
+        <v>956</v>
+      </c>
+      <c r="P44" s="6" t="s">
+        <v>957</v>
+      </c>
+      <c r="Q44" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
+        <v>43</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>958</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>959</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>960</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H45" s="6">
+        <v>1</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L45" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M45" s="6" t="s">
+        <v>961</v>
+      </c>
+      <c r="N45" s="6" t="s">
+        <v>962</v>
+      </c>
+      <c r="O45" s="6" t="s">
+        <v>963</v>
+      </c>
+      <c r="P45" s="6" t="s">
+        <v>964</v>
+      </c>
+      <c r="Q45" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
+        <v>44</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>965</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>966</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>967</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H46" s="6">
+        <v>1</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L46" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M46" s="6" t="s">
+        <v>968</v>
+      </c>
+      <c r="N46" s="6" t="s">
+        <v>969</v>
+      </c>
+      <c r="O46" s="6" t="s">
+        <v>970</v>
+      </c>
+      <c r="P46" s="6" t="s">
+        <v>971</v>
+      </c>
+      <c r="Q46" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="6">
+        <v>45</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>972</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>973</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>974</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H47" s="6">
+        <v>1</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L47" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M47" s="6" t="s">
+        <v>975</v>
+      </c>
+      <c r="N47" s="6" t="s">
+        <v>976</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>977</v>
+      </c>
+      <c r="P47" s="6" t="s">
+        <v>978</v>
+      </c>
+      <c r="Q47" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="6">
+        <v>46</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>979</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>980</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>981</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H48" s="6">
+        <v>1</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L48" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M48" s="6" t="s">
+        <v>982</v>
+      </c>
+      <c r="N48" s="6" t="s">
+        <v>983</v>
+      </c>
+      <c r="O48" s="6" t="s">
+        <v>984</v>
+      </c>
+      <c r="P48" s="6" t="s">
+        <v>985</v>
+      </c>
+      <c r="Q48" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="6">
+        <v>47</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>986</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>987</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>988</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H49" s="6">
+        <v>1</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L49" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M49" s="6" t="s">
+        <v>989</v>
+      </c>
+      <c r="N49" s="6" t="s">
+        <v>990</v>
+      </c>
+      <c r="O49" s="6" t="s">
+        <v>991</v>
+      </c>
+      <c r="P49" s="6" t="s">
+        <v>992</v>
+      </c>
+      <c r="Q49" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="6">
+        <v>48</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>993</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>994</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>995</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H50" s="6">
+        <v>1</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>904</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L50" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M50" s="6" t="s">
+        <v>996</v>
+      </c>
+      <c r="N50" s="6" t="s">
+        <v>997</v>
+      </c>
+      <c r="O50" s="6" t="s">
+        <v>998</v>
+      </c>
+      <c r="P50" s="6" t="s">
+        <v>999</v>
+      </c>
+      <c r="Q50" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="6">
+        <v>49</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H51" s="6">
+        <v>1</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L51" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M51" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N51" s="6" t="s">
+        <v>1004</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>1005</v>
+      </c>
+      <c r="P51" s="6" t="s">
+        <v>1006</v>
+      </c>
+      <c r="Q51" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="6">
+        <v>50</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H52" s="6">
+        <v>1</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L52" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M52" s="6" t="s">
+        <v>1010</v>
+      </c>
+      <c r="N52" s="6" t="s">
+        <v>1011</v>
+      </c>
+      <c r="O52" s="6" t="s">
+        <v>1012</v>
+      </c>
+      <c r="P52" s="6" t="s">
+        <v>1013</v>
+      </c>
+      <c r="Q52" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="6">
+        <v>51</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H53" s="6">
+        <v>1</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J53" s="6" t="s">
+        <v>1017</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L53" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M53" s="6" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N53" s="6" t="s">
+        <v>1019</v>
+      </c>
+      <c r="O53" s="6" t="s">
+        <v>1020</v>
+      </c>
+      <c r="P53" s="6" t="s">
+        <v>1021</v>
+      </c>
+      <c r="Q53" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="6">
+        <v>52</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H54" s="6">
+        <v>1</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L54" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M54" s="6" t="s">
+        <v>1026</v>
+      </c>
+      <c r="N54" s="6" t="s">
+        <v>1027</v>
+      </c>
+      <c r="O54" s="6" t="s">
+        <v>1028</v>
+      </c>
+      <c r="P54" s="6" t="s">
+        <v>1029</v>
+      </c>
+      <c r="Q54" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A55" s="6">
+        <v>53</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H55" s="6">
+        <v>1</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L55" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M55" s="6" t="s">
+        <v>1033</v>
+      </c>
+      <c r="N55" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>1034</v>
+      </c>
+      <c r="P55" s="6" t="s">
+        <v>1035</v>
+      </c>
+      <c r="Q55" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A56" s="6">
+        <v>54</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H56" s="6">
+        <v>1</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K56" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L56" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M56" s="6" t="s">
+        <v>1039</v>
+      </c>
+      <c r="N56" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="O56" s="6" t="s">
+        <v>1040</v>
+      </c>
+      <c r="P56" s="6" t="s">
+        <v>1041</v>
+      </c>
+      <c r="Q56" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="6">
+        <v>55</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H57" s="6">
+        <v>1</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>1045</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>1046</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L57" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M57" s="6" t="s">
+        <v>1047</v>
+      </c>
+      <c r="N57" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="O57" s="6" t="s">
+        <v>1048</v>
+      </c>
+      <c r="P57" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="Q57" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="6">
+        <v>56</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H58" s="6">
+        <v>1</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>1053</v>
+      </c>
+      <c r="J58" s="6" t="s">
+        <v>1054</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L58" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M58" s="6" t="s">
+        <v>1055</v>
+      </c>
+      <c r="N58" s="6" t="s">
+        <v>1056</v>
+      </c>
+      <c r="O58" s="6" t="s">
+        <v>1057</v>
+      </c>
+      <c r="P58" s="6" t="s">
+        <v>1058</v>
+      </c>
+      <c r="Q58" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="6">
+        <v>57</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>1061</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H59" s="6">
+        <v>1</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J59" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K59" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L59" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M59" s="6" t="s">
+        <v>1062</v>
+      </c>
+      <c r="N59" s="6" t="s">
+        <v>1063</v>
+      </c>
+      <c r="O59" s="6" t="s">
+        <v>1064</v>
+      </c>
+      <c r="P59" s="6" t="s">
+        <v>1065</v>
+      </c>
+      <c r="Q59" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="6">
+        <v>58</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H60" s="6">
+        <v>1</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J60" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L60" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M60" s="6" t="s">
+        <v>1069</v>
+      </c>
+      <c r="N60" s="6" t="s">
+        <v>1070</v>
+      </c>
+      <c r="O60" s="6" t="s">
+        <v>1071</v>
+      </c>
+      <c r="P60" s="6" t="s">
+        <v>1072</v>
+      </c>
+      <c r="Q60" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="6">
+        <v>59</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>1076</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H61" s="6">
+        <v>1</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J61" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K61" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L61" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M61" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="N61" s="6" t="s">
+        <v>1078</v>
+      </c>
+      <c r="O61" s="6" t="s">
+        <v>1079</v>
+      </c>
+      <c r="P61" s="6" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Q61" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A62" s="6">
+        <v>60</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H62" s="6">
+        <v>1</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J62" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="K62" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L62" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M62" s="6" t="s">
+        <v>1085</v>
+      </c>
+      <c r="N62" s="6" t="s">
+        <v>1086</v>
+      </c>
+      <c r="O62" s="6" t="s">
+        <v>1087</v>
+      </c>
+      <c r="P62" s="6" t="s">
+        <v>1088</v>
+      </c>
+      <c r="Q62" s="6" t="s">
         <v>658</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add the test cases 60-100 for limit module
</commit_message>
<xml_diff>
--- a/limits.xlsx
+++ b/limits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed.El-Sawy\Documents\hdb_test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD3F4BB-D917-4FAD-92BA-5883A82C0D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C27F52-450E-48ED-AE53-B5D2B63630CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3D412268-5103-411D-BBE4-3652EEC1385B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2771" uniqueCount="1363">
   <si>
     <t>Limit</t>
   </si>
@@ -6461,11 +6461,6 @@
     <t>Verify auto-numbering sequence for multiple limits without collateral</t>
   </si>
   <si>
-    <t>1. Login as Maker 
-2. Create multiple unsecured limits 
-3. Check limit IDs</t>
-  </si>
-  <si>
     <t>1. Maker logged in 
 2. IDs auto-increment as expected</t>
   </si>
@@ -6580,57 +6575,879 @@
     <t>System allows edits before execution</t>
   </si>
   <si>
-    <t>LIM-59</t>
-  </si>
-  <si>
-    <t>limit_post_usage_field_auto_update_maker</t>
-  </si>
-  <si>
-    <t>Verify automatic field update after limit usage</t>
-  </si>
-  <si>
-    <t>Limit must be created and used</t>
-  </si>
-  <si>
-    <t>1. Use limit partially 
-2. Review auto-filled fields</t>
-  </si>
-  <si>
-    <t>Fields: Used Amount, Available Amount, Guarantee No., Limit ID, Limit Type</t>
-  </si>
-  <si>
-    <t>1. Fields updated as per usage</t>
-  </si>
-  <si>
-    <t>Fields update automatically after usage</t>
-  </si>
-  <si>
-    <t>LIM-60</t>
-  </si>
-  <si>
-    <t>limit_search_existing_limit_inquiry_maker</t>
-  </si>
-  <si>
-    <t>Verify inquiry screen displays all expected data</t>
-  </si>
-  <si>
     <t>Limit must be created</t>
   </si>
   <si>
     <t>1. Login as Maker 
-2. Search by limit ID 
-3. Confirm field values</t>
-  </si>
-  <si>
-    <t>Limit ID: LIM01234</t>
-  </si>
-  <si>
-    <t>1. Maker logged in 
-2. Fields populated 
-3. Values match what was entered</t>
-  </si>
-  <si>
-    <t>Inquiry screen data is consistent</t>
+2. Create multiple unsecured limits 
+3. Check limit Ids</t>
+  </si>
+  <si>
+    <t>LIM-61</t>
+  </si>
+  <si>
+    <t>limit_maximum_amount_validation_input_with_collateral_maker</t>
+  </si>
+  <si>
+    <t>Validate maximum limit amount for collateral</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Navigate to LIMIT.INPUT &gt; 3. Enter maximum allowed limit amount &gt; 4. Submit</t>
+  </si>
+  <si>
+    <t>Limit Amount: 99999999</t>
+  </si>
+  <si>
+    <t>1. Maker logged in &gt; 2. Screen accessed &gt; 3. Maximum value entered &gt; 4. Submission accepted</t>
+  </si>
+  <si>
+    <t>System accepts up to the allowed maximum amount</t>
+  </si>
+  <si>
+    <t>LIM-62</t>
+  </si>
+  <si>
+    <t>limit_maximum_amount_validation_input_without_collateral_maker</t>
+  </si>
+  <si>
+    <t>Validate maximum limit amount without collateral</t>
+  </si>
+  <si>
+    <t>System accepts the value as it's within max allowed</t>
+  </si>
+  <si>
+    <t>LIM-63</t>
+  </si>
+  <si>
+    <t>limit_minimum_amount_validation_input_with_collateral_maker</t>
+  </si>
+  <si>
+    <t>Validate minimum limit amount for collateral</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Navigate to LIMIT.INPUT &gt; 3. Enter amount below minimum &gt; 4. Submit</t>
+  </si>
+  <si>
+    <t>Limit Amount: 10</t>
+  </si>
+  <si>
+    <t>1. Maker logged in &gt; 2. Screen accessed &gt; 3. Amount entered below threshold &gt; 4. Submission rejected</t>
+  </si>
+  <si>
+    <t>System rejects values below minimum allowed</t>
+  </si>
+  <si>
+    <t>LIM-64</t>
+  </si>
+  <si>
+    <t>limit_minimum_amount_validation_input_without_collateral_maker</t>
+  </si>
+  <si>
+    <t>Validate minimum limit amount without collateral</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Navigate to LIMIT.INPUT &gt; 3. Enter value under allowed minimum &gt; 4. Submit</t>
+  </si>
+  <si>
+    <t>Limit Amount: 50</t>
+  </si>
+  <si>
+    <t>1. Maker logged in &gt; 2. Screen accessed &gt; 3. Minimum value entered &gt; 4. Submission blocked</t>
+  </si>
+  <si>
+    <t>System blocks amount under minimum limit</t>
+  </si>
+  <si>
+    <t>LIM-65</t>
+  </si>
+  <si>
+    <t>limit_invalid_currency_input_maker</t>
+  </si>
+  <si>
+    <t>Attempt to create limit with invalid currency</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Enter invalid currency &gt; 3. Try to submit</t>
+  </si>
+  <si>
+    <t>Currency: XYZ</t>
+  </si>
+  <si>
+    <t>1. Maker logged in &gt; 2. Invalid currency entered &gt; 3. Error message displayed</t>
+  </si>
+  <si>
+    <t>System rejects invalid currency input</t>
+  </si>
+  <si>
+    <t>LIM-66</t>
+  </si>
+  <si>
+    <t>limit_duplicate_limit_id_maker</t>
+  </si>
+  <si>
+    <t>Try to create limit with existing ID</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Use existing Limit ID &gt; 3. Submit</t>
+  </si>
+  <si>
+    <t>Limit ID: LIM00001</t>
+  </si>
+  <si>
+    <t>1. Maker entered duplicate ID &gt; 2. Submission blocked</t>
+  </si>
+  <si>
+    <t>Error: Duplicate limit ID not allowed</t>
+  </si>
+  <si>
+    <t>LIM-67</t>
+  </si>
+  <si>
+    <t>limit_negative_amount_entry_maker</t>
+  </si>
+  <si>
+    <t>Attempt to input negative limit amount</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Enter negative amount &gt; 3. Submit</t>
+  </si>
+  <si>
+    <t>Amount: -50000</t>
+  </si>
+  <si>
+    <t>1. Negative value entered &gt; 2. Error displayed &gt; 3. Submission rejected</t>
+  </si>
+  <si>
+    <t>System blocks negative amounts</t>
+  </si>
+  <si>
+    <t>LIM-68</t>
+  </si>
+  <si>
+    <t>limit_zero_amount_entry_maker</t>
+  </si>
+  <si>
+    <t>Attempt to create limit with amount = 0</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Enter amount = 0 &gt; 3. Submit</t>
+  </si>
+  <si>
+    <t>Amount: 0</t>
+  </si>
+  <si>
+    <t>1. Zero amount submitted &gt; 2. Error triggered &gt; 3. Record not saved</t>
+  </si>
+  <si>
+    <t>System enforces positive amounts</t>
+  </si>
+  <si>
+    <t>LIM-69</t>
+  </si>
+  <si>
+    <t>limit_missing_mandatory_fields_maker</t>
+  </si>
+  <si>
+    <t>Submit form with missing mandatory fields</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Leave required fields blank &gt; 3. Submit</t>
+  </si>
+  <si>
+    <t>Blank Approval Date, Amount</t>
+  </si>
+  <si>
+    <t>1. Submission blocked &gt; 2. System displays mandatory field error</t>
+  </si>
+  <si>
+    <t>Error: Required fields missing</t>
+  </si>
+  <si>
+    <t>LIM-70</t>
+  </si>
+  <si>
+    <t>limit_invalid_date_format_maker</t>
+  </si>
+  <si>
+    <t>Enter invalid date format in approval field</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Enter invalid date &gt; 3. Submit</t>
+  </si>
+  <si>
+    <t>Approval Date: 99/99/9999</t>
+  </si>
+  <si>
+    <t>1. Maker entered invalid format &gt; 2. Error displayed</t>
+  </si>
+  <si>
+    <t>System rejects incorrect date formats</t>
+  </si>
+  <si>
+    <t>LIM-71</t>
+  </si>
+  <si>
+    <t>limit_maximum_limit_value_maker</t>
+  </si>
+  <si>
+    <t>Create limit with maximum allowed value</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Enter max value &gt; 3. Submit</t>
+  </si>
+  <si>
+    <t>Amount: 999999999</t>
+  </si>
+  <si>
+    <t>1. Maker submitted &gt; 2. Limit accepted</t>
+  </si>
+  <si>
+    <t>Max value accepted and saved</t>
+  </si>
+  <si>
+    <t>LIM-72</t>
+  </si>
+  <si>
+    <t>limit_exceed_maximum_limit_value_maker</t>
+  </si>
+  <si>
+    <t>Attempt to exceed allowed limit value</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Enter amount above max &gt; 3. Submit</t>
+  </si>
+  <si>
+    <t>Amount: 1000000000</t>
+  </si>
+  <si>
+    <t>1. Maker submitted &gt; 2. System rejected submission</t>
+  </si>
+  <si>
+    <t>Error: Maximum limit exceeded</t>
+  </si>
+  <si>
+    <t>LIM-73</t>
+  </si>
+  <si>
+    <t>limit_inquiry_existing_limit_data_maker</t>
+  </si>
+  <si>
+    <t>Inquire data for approved limit</t>
+  </si>
+  <si>
+    <t>Limit must be approved</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Search by Limit ID &gt; 3. View details</t>
+  </si>
+  <si>
+    <t>Limit ID: LIM00055</t>
+  </si>
+  <si>
+    <t>1. Inquiry successful &gt; 2. All fields displayed</t>
+  </si>
+  <si>
+    <t>Approved limit details visible</t>
+  </si>
+  <si>
+    <t>LIM-74</t>
+  </si>
+  <si>
+    <t>limit_search_by_customer_id_maker</t>
+  </si>
+  <si>
+    <t>Search limits by customer ID</t>
+  </si>
+  <si>
+    <t>Limit must exist for customer</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Search using customer ID &gt; 3. Review results</t>
+  </si>
+  <si>
+    <t>Customer ID: CUST123456</t>
+  </si>
+  <si>
+    <t>1. System returned all matching records</t>
+  </si>
+  <si>
+    <t>Search filter by customer ID working</t>
+  </si>
+  <si>
+    <t>LIM-75</t>
+  </si>
+  <si>
+    <t>limit_expired_limit_not_editable_maker</t>
+  </si>
+  <si>
+    <t>Try editing expired limit</t>
+  </si>
+  <si>
+    <t>Limit must be expired</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Select expired limit &gt; 3. Try to edit</t>
+  </si>
+  <si>
+    <t>Expired Limit ID: LIM00020</t>
+  </si>
+  <si>
+    <t>1. Maker unable to edit expired record</t>
+  </si>
+  <si>
+    <t>Error: Expired limits cannot be edited</t>
+  </si>
+  <si>
+    <t>LIM-76</t>
+  </si>
+  <si>
+    <t>limit_review_cycle_enforcement_maker</t>
+  </si>
+  <si>
+    <t>Review cycle must be selected for secured limit</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Enter secured limit &gt; 3. Leave review cycle blank &gt; 4. Submit</t>
+  </si>
+  <si>
+    <t>1. Maker submitted &gt; 2. System blocked &gt; 3. Error for missing review cycle</t>
+  </si>
+  <si>
+    <t>Error displayed for missing review cycle</t>
+  </si>
+  <si>
+    <t>LIM-77</t>
+  </si>
+  <si>
+    <t>limit_date_validation_future_date_maker</t>
+  </si>
+  <si>
+    <t>Use future date in approval</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Set future date &gt; 3. Submit</t>
+  </si>
+  <si>
+    <t>Approval Date: 31.12.2030</t>
+  </si>
+  <si>
+    <t>1. Submission successful if date accepted</t>
+  </si>
+  <si>
+    <t>Future date accepted if within valid range</t>
+  </si>
+  <si>
+    <t>LIM-78</t>
+  </si>
+  <si>
+    <t>limit_currency_field_validation_maker</t>
+  </si>
+  <si>
+    <t>Check currency field dropdown values</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Open Currency dropdown &gt; 3. Review values</t>
+  </si>
+  <si>
+    <t>1. Dropdown shows active currencies only</t>
+  </si>
+  <si>
+    <t>Only valid currencies are selectable</t>
+  </si>
+  <si>
+    <t>LIM-79</t>
+  </si>
+  <si>
+    <t>limit_validate_first_grant_date_maker</t>
+  </si>
+  <si>
+    <t>Check First Grant Date logic</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Enter earlier date &gt; 3. Submit</t>
+  </si>
+  <si>
+    <t>First Grant Date: 01.01.2010</t>
+  </si>
+  <si>
+    <t>1. Submission accepted if date before approval</t>
+  </si>
+  <si>
+    <t>First Grant must be before or same as approval</t>
+  </si>
+  <si>
+    <t>LIM-80</t>
+  </si>
+  <si>
+    <t>limit_cancel_pending_limit_checker</t>
+  </si>
+  <si>
+    <t>Cancel pending limit from checker queue</t>
+  </si>
+  <si>
+    <t>Limit must be submitted by maker</t>
+  </si>
+  <si>
+    <t>1. Login as Checker &gt; 2. View pending record &gt; 3. Cancel</t>
+  </si>
+  <si>
+    <t>Limit ID: LIM00070</t>
+  </si>
+  <si>
+    <t>1. Record status updated to cancelled</t>
+  </si>
+  <si>
+    <t>Cancellation processed correctly</t>
+  </si>
+  <si>
+    <t>LIM-81</t>
+  </si>
+  <si>
+    <t>limit_validate_collateral_amount_vs_limit_maker</t>
+  </si>
+  <si>
+    <t>Collateral must be &gt;= limit amount</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Enter collateral lower than limit &gt; 3. Submit</t>
+  </si>
+  <si>
+    <t>Collateral: 20000; Limit: 50000</t>
+  </si>
+  <si>
+    <t>1. System prevents submission &gt; 2. Error displayed</t>
+  </si>
+  <si>
+    <t>Error: Collateral less than limit not allowed</t>
+  </si>
+  <si>
+    <t>LIM-82</t>
+  </si>
+  <si>
+    <t>limit_currency_exchange_check_maker</t>
+  </si>
+  <si>
+    <t>Verify currency conversion on foreign limit</t>
+  </si>
+  <si>
+    <t>Exchange rates must be setup</t>
+  </si>
+  <si>
+    <t>1. Enter limit in USD &gt; 2. Confirm conversion to EGP</t>
+  </si>
+  <si>
+    <t>Amount: 10000 USD</t>
+  </si>
+  <si>
+    <t>1. System calculates correct equivalent EGP</t>
+  </si>
+  <si>
+    <t>Currency exchange reflected accurately</t>
+  </si>
+  <si>
+    <t>LIM-83</t>
+  </si>
+  <si>
+    <t>limit_reactivate_cancelled_limit_checker</t>
+  </si>
+  <si>
+    <t>Re-approve a cancelled limit</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Must have a previously cancelled limit</t>
+  </si>
+  <si>
+    <t>1. Login as Checker &gt; 2. Search cancelled limit &gt; 3. Re-authorize</t>
+  </si>
+  <si>
+    <t>Cancelled Limit ID</t>
+  </si>
+  <si>
+    <t>1. System updates status to active</t>
+  </si>
+  <si>
+    <t>Cancelled limit reactivated</t>
+  </si>
+  <si>
+    <t>LIM-84</t>
+  </si>
+  <si>
+    <t>limit_auto_limit_name_population_maker</t>
+  </si>
+  <si>
+    <t>Check auto generation of limit name</t>
+  </si>
+  <si>
+    <t>1. Login as Maker &gt; 2. Select customer &gt; 3. Observe limit name field</t>
+  </si>
+  <si>
+    <t>1. Limit name auto-filled based on rules</t>
+  </si>
+  <si>
+    <t>Auto name generation working as per logic</t>
+  </si>
+  <si>
+    <t>LIM-85</t>
+  </si>
+  <si>
+    <t>limit_duplicate_checker_approval_checker</t>
+  </si>
+  <si>
+    <t>Checker tries to approve same record twice</t>
+  </si>
+  <si>
+    <t>Limit must be pending</t>
+  </si>
+  <si>
+    <t>1. Approve once &gt; 2. Try to approve again</t>
+  </si>
+  <si>
+    <t>Limit ID: LIM00077</t>
+  </si>
+  <si>
+    <t>1. System blocks second approval attempt</t>
+  </si>
+  <si>
+    <t>Error: Already approved</t>
+  </si>
+  <si>
+    <t>LIM-86</t>
+  </si>
+  <si>
+    <t>limit_customer_blacklist_validation_maker</t>
+  </si>
+  <si>
+    <t>Prevent limit creation for blacklisted customer</t>
+  </si>
+  <si>
+    <t>Customer must be flagged</t>
+  </si>
+  <si>
+    <t>1. Enter blacklisted customer &gt; 2. Try to submit</t>
+  </si>
+  <si>
+    <t>Customer ID: CUST99999</t>
+  </si>
+  <si>
+    <t>1. Submission blocked &gt; 2. Error shown</t>
+  </si>
+  <si>
+    <t>Error: Blacklisted customer not allowed</t>
+  </si>
+  <si>
+    <t>LIM-87</t>
+  </si>
+  <si>
+    <t>limit_guarantee_type_mandatory_for_secured_maker</t>
+  </si>
+  <si>
+    <t>Check guarantee type is mandatory for secured limits</t>
+  </si>
+  <si>
+    <t>1. Create secured limit &gt; 2. Leave guarantee blank &gt; 3. Submit</t>
+  </si>
+  <si>
+    <t>Limit Type: Secured</t>
+  </si>
+  <si>
+    <t>1. Error message for missing guarantee</t>
+  </si>
+  <si>
+    <t>Error: Guarantee type required for secured limit</t>
+  </si>
+  <si>
+    <t>LIM-88</t>
+  </si>
+  <si>
+    <t>limit_link_multiple_accounts_to_limit_maker</t>
+  </si>
+  <si>
+    <t>Link more than one account to a single limit</t>
+  </si>
+  <si>
+    <t>1. Select limit &gt; 2. Link to multiple accounts</t>
+  </si>
+  <si>
+    <t>Accounts: 12345, 67890</t>
+  </si>
+  <si>
+    <t>1. All accounts linked to same limit</t>
+  </si>
+  <si>
+    <t>Multiple links created successfully</t>
+  </si>
+  <si>
+    <t>LIM-89</t>
+  </si>
+  <si>
+    <t>limit_remove_account_linked_to_limit_maker</t>
+  </si>
+  <si>
+    <t>Remove an account already linked to limit</t>
+  </si>
+  <si>
+    <t>Account must be linked first</t>
+  </si>
+  <si>
+    <t>1. Select linked account &gt; 2. Remove &gt; 3. Submit</t>
+  </si>
+  <si>
+    <t>Account ID: 12345</t>
+  </si>
+  <si>
+    <t>1. Account unlinked successfully</t>
+  </si>
+  <si>
+    <t>Account removed from limit</t>
+  </si>
+  <si>
+    <t>LIM-90</t>
+  </si>
+  <si>
+    <t>limit_validate_authorized_vs_used_maker</t>
+  </si>
+  <si>
+    <t>Verify used amount doesn't exceed authorized</t>
+  </si>
+  <si>
+    <t>Limit must be used partially</t>
+  </si>
+  <si>
+    <t>1. Check Authorized vs Used</t>
+  </si>
+  <si>
+    <t>Authorized: 50000; Used: 52000</t>
+  </si>
+  <si>
+    <t>1. Error triggered &gt; 2. Usage blocked</t>
+  </si>
+  <si>
+    <t>Error: Usage exceeds authorized amount</t>
+  </si>
+  <si>
+    <t>LIM-91</t>
+  </si>
+  <si>
+    <t>limit_partial_amendment_maker</t>
+  </si>
+  <si>
+    <t>Amend only selected fields in limit</t>
+  </si>
+  <si>
+    <t>Limit must exist</t>
+  </si>
+  <si>
+    <t>1. Change Review Cycle only &gt; 2. Submit</t>
+  </si>
+  <si>
+    <t>New Review Cycle: 6 Months</t>
+  </si>
+  <si>
+    <t>1. Amendment saved successfully</t>
+  </si>
+  <si>
+    <t>Partial amendments allowed</t>
+  </si>
+  <si>
+    <t>LIM-92</t>
+  </si>
+  <si>
+    <t>limit_validate_expiry_before_review_maker</t>
+  </si>
+  <si>
+    <t>Check expiry date is after review date</t>
+  </si>
+  <si>
+    <t>1. Set Expiry &lt; Review Date &gt; 2. Submit</t>
+  </si>
+  <si>
+    <t>Expiry: 01.01.2026; Review: 01.01.2027</t>
+  </si>
+  <si>
+    <t>1. System shows validation error</t>
+  </si>
+  <si>
+    <t>Error: Expiry must be after review</t>
+  </si>
+  <si>
+    <t>LIM-93</t>
+  </si>
+  <si>
+    <t>limit_input_with_special_characters_maker</t>
+  </si>
+  <si>
+    <t>Attempt to enter special chars in description field</t>
+  </si>
+  <si>
+    <t>1. Enter special characters &gt; 2. Submit</t>
+  </si>
+  <si>
+    <t>Description: @#$%&amp;*</t>
+  </si>
+  <si>
+    <t>1. System either blocks or sanitizes input</t>
+  </si>
+  <si>
+    <t>Special character handling verified</t>
+  </si>
+  <si>
+    <t>LIM-94</t>
+  </si>
+  <si>
+    <t>limit_field_length_validation_maker</t>
+  </si>
+  <si>
+    <t>Check max character limits in fields</t>
+  </si>
+  <si>
+    <t>1. Enter long string &gt; 2. Submit</t>
+  </si>
+  <si>
+    <t>Description: 300 characters</t>
+  </si>
+  <si>
+    <t>1. System trims or blocks excess characters</t>
+  </si>
+  <si>
+    <t>Field length validation applied</t>
+  </si>
+  <si>
+    <t>LIM-95</t>
+  </si>
+  <si>
+    <t>limit_checker_reject_reason_mandatory_checker</t>
+  </si>
+  <si>
+    <t>Checker must enter reason on rejection</t>
+  </si>
+  <si>
+    <t>1. Reject limit &gt; 2. Leave reason blank &gt; 3. Submit</t>
+  </si>
+  <si>
+    <t>1. System blocks rejection without reason</t>
+  </si>
+  <si>
+    <t>Error: Rejection reason required</t>
+  </si>
+  <si>
+    <t>LIM-96</t>
+  </si>
+  <si>
+    <t>limit_create_for_different_branch_maker</t>
+  </si>
+  <si>
+    <t>Create limit from another branch than the account</t>
+  </si>
+  <si>
+    <t>Branches must exist</t>
+  </si>
+  <si>
+    <t>1. Enter account in branch A &gt; 2. Create limit from branch B</t>
+  </si>
+  <si>
+    <t>Account Branch: 001; Maker Branch: 002</t>
+  </si>
+  <si>
+    <t>1. System accepts or flags based on rule</t>
+  </si>
+  <si>
+    <t>Cross-branch creation validated</t>
+  </si>
+  <si>
+    <t>LIM-97</t>
+  </si>
+  <si>
+    <t>limit_authorized_vs_utilized_ratio_validation_maker</t>
+  </si>
+  <si>
+    <t>Check utilization percentage does not exceed threshold</t>
+  </si>
+  <si>
+    <t>1. Check utilization &gt; 2. Submit</t>
+  </si>
+  <si>
+    <t>Authorized: 100000; Used: 95000 (95%)</t>
+  </si>
+  <si>
+    <t>1. System allows if below threshold</t>
+  </si>
+  <si>
+    <t>Ratio enforcement confirmed</t>
+  </si>
+  <si>
+    <t>LIM-98</t>
+  </si>
+  <si>
+    <t>limit_overdue_review_date_alert_maker</t>
+  </si>
+  <si>
+    <t>Alert for overdue review date</t>
+  </si>
+  <si>
+    <t>Review date in past</t>
+  </si>
+  <si>
+    <t>1. Enter past review date &gt; 2. Submit</t>
+  </si>
+  <si>
+    <t>Review Date: 01.01.2024</t>
+  </si>
+  <si>
+    <t>1. System triggers overdue alert</t>
+  </si>
+  <si>
+    <t>Review alert shown correctly</t>
+  </si>
+  <si>
+    <t>LIM-99</t>
+  </si>
+  <si>
+    <t>limit_edit_limit_type_post_creation_maker</t>
+  </si>
+  <si>
+    <t>Try to change limit type after creation</t>
+  </si>
+  <si>
+    <t>1. Attempt to change limit type &gt; 2. Submit</t>
+  </si>
+  <si>
+    <t>Old Type: Secured &gt; New Type: Unsecured</t>
+  </si>
+  <si>
+    <t>1. System prevents edit of limit type</t>
+  </si>
+  <si>
+    <t>Error: Limit type cannot be changed post creation</t>
+  </si>
+  <si>
+    <t>LIM-100</t>
+  </si>
+  <si>
+    <t>limit_clone_existing_limit_maker</t>
+  </si>
+  <si>
+    <t>Clone a limit using existing record as template</t>
+  </si>
+  <si>
+    <t>Existing limit required</t>
+  </si>
+  <si>
+    <t>1. Select existing limit &gt; 2. Clone &gt; 3. Modify as needed &gt; 4. Submit</t>
+  </si>
+  <si>
+    <t>Template: LIM00050</t>
+  </si>
+  <si>
+    <t>1. New record created based on template</t>
+  </si>
+  <si>
+    <t>Limit cloned successfully</t>
   </si>
 </sst>
 </file>
@@ -11644,10 +12461,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB919F80-9B96-4E34-ADD6-E7884B62F830}">
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="51.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14625,16 +15442,16 @@
         <v>45823</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>1039</v>
+        <v>1073</v>
       </c>
       <c r="N56" s="6" t="s">
         <v>658</v>
       </c>
       <c r="O56" s="6" t="s">
+        <v>1039</v>
+      </c>
+      <c r="P56" s="6" t="s">
         <v>1040</v>
-      </c>
-      <c r="P56" s="6" t="s">
-        <v>1041</v>
       </c>
       <c r="Q56" s="6" t="s">
         <v>658</v>
@@ -14645,13 +15462,13 @@
         <v>55</v>
       </c>
       <c r="B57" s="6" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>1042</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="D57" s="6" t="s">
         <v>1043</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>1044</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>3</v>
@@ -14666,10 +15483,10 @@
         <v>1</v>
       </c>
       <c r="I57" s="6" t="s">
+        <v>1044</v>
+      </c>
+      <c r="J57" s="6" t="s">
         <v>1045</v>
-      </c>
-      <c r="J57" s="6" t="s">
-        <v>1046</v>
       </c>
       <c r="K57" s="6" t="s">
         <v>0</v>
@@ -14678,16 +15495,16 @@
         <v>45823</v>
       </c>
       <c r="M57" s="6" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="N57" s="6" t="s">
         <v>658</v>
       </c>
       <c r="O57" s="6" t="s">
+        <v>1047</v>
+      </c>
+      <c r="P57" s="6" t="s">
         <v>1048</v>
-      </c>
-      <c r="P57" s="6" t="s">
-        <v>1049</v>
       </c>
       <c r="Q57" s="6" t="s">
         <v>658</v>
@@ -14698,13 +15515,13 @@
         <v>56</v>
       </c>
       <c r="B58" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C58" s="6" t="s">
         <v>1050</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="D58" s="6" t="s">
         <v>1051</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>1052</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>3</v>
@@ -14719,10 +15536,10 @@
         <v>1</v>
       </c>
       <c r="I58" s="6" t="s">
+        <v>1052</v>
+      </c>
+      <c r="J58" s="6" t="s">
         <v>1053</v>
-      </c>
-      <c r="J58" s="6" t="s">
-        <v>1054</v>
       </c>
       <c r="K58" s="6" t="s">
         <v>0</v>
@@ -14731,16 +15548,16 @@
         <v>45823</v>
       </c>
       <c r="M58" s="6" t="s">
+        <v>1054</v>
+      </c>
+      <c r="N58" s="6" t="s">
         <v>1055</v>
       </c>
-      <c r="N58" s="6" t="s">
+      <c r="O58" s="6" t="s">
         <v>1056</v>
       </c>
-      <c r="O58" s="6" t="s">
+      <c r="P58" s="6" t="s">
         <v>1057</v>
-      </c>
-      <c r="P58" s="6" t="s">
-        <v>1058</v>
       </c>
       <c r="Q58" s="6" t="s">
         <v>658</v>
@@ -14751,13 +15568,13 @@
         <v>57</v>
       </c>
       <c r="B59" s="6" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>1059</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="D59" s="6" t="s">
         <v>1060</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>1061</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>3</v>
@@ -14784,16 +15601,16 @@
         <v>45823</v>
       </c>
       <c r="M59" s="6" t="s">
+        <v>1061</v>
+      </c>
+      <c r="N59" s="6" t="s">
         <v>1062</v>
       </c>
-      <c r="N59" s="6" t="s">
+      <c r="O59" s="6" t="s">
         <v>1063</v>
       </c>
-      <c r="O59" s="6" t="s">
+      <c r="P59" s="6" t="s">
         <v>1064</v>
-      </c>
-      <c r="P59" s="6" t="s">
-        <v>1065</v>
       </c>
       <c r="Q59" s="6" t="s">
         <v>658</v>
@@ -14804,13 +15621,13 @@
         <v>58</v>
       </c>
       <c r="B60" s="6" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C60" s="6" t="s">
         <v>1066</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="D60" s="6" t="s">
         <v>1067</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>1068</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>3</v>
@@ -14837,39 +15654,39 @@
         <v>45823</v>
       </c>
       <c r="M60" s="6" t="s">
+        <v>1068</v>
+      </c>
+      <c r="N60" s="6" t="s">
         <v>1069</v>
       </c>
-      <c r="N60" s="6" t="s">
+      <c r="O60" s="6" t="s">
         <v>1070</v>
       </c>
-      <c r="O60" s="6" t="s">
+      <c r="P60" s="6" t="s">
         <v>1071</v>
-      </c>
-      <c r="P60" s="6" t="s">
-        <v>1072</v>
       </c>
       <c r="Q60" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>3</v>
+        <v>1077</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>1076</v>
+        <v>654</v>
       </c>
       <c r="G61" s="6" t="s">
         <v>654</v>
@@ -14890,39 +15707,39 @@
         <v>45823</v>
       </c>
       <c r="M61" s="6" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="N61" s="6" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="O61" s="6" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="P61" s="6" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="Q61" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>3</v>
+        <v>1077</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>1084</v>
+        <v>654</v>
       </c>
       <c r="G62" s="6" t="s">
         <v>654</v>
@@ -14934,7 +15751,7 @@
         <v>655</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>663</v>
+        <v>870</v>
       </c>
       <c r="K62" s="6" t="s">
         <v>0</v>
@@ -14943,18 +15760,2032 @@
         <v>45823</v>
       </c>
       <c r="M62" s="6" t="s">
+        <v>1078</v>
+      </c>
+      <c r="N62" s="6" t="s">
+        <v>1079</v>
+      </c>
+      <c r="O62" s="6" t="s">
+        <v>1080</v>
+      </c>
+      <c r="P62" s="6" t="s">
         <v>1085</v>
       </c>
-      <c r="N62" s="6" t="s">
+      <c r="Q62" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A63" s="6">
+        <v>63</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>1086</v>
       </c>
-      <c r="O62" s="6" t="s">
+      <c r="C63" s="6" t="s">
         <v>1087</v>
       </c>
-      <c r="P62" s="6" t="s">
+      <c r="D63" s="6" t="s">
         <v>1088</v>
       </c>
-      <c r="Q62" s="6" t="s">
+      <c r="E63" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H63" s="6">
+        <v>1</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J63" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K63" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L63" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M63" s="6" t="s">
+        <v>1089</v>
+      </c>
+      <c r="N63" s="6" t="s">
+        <v>1090</v>
+      </c>
+      <c r="O63" s="6" t="s">
+        <v>1091</v>
+      </c>
+      <c r="P63" s="6" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Q63" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A64" s="6">
+        <v>64</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H64" s="6">
+        <v>1</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L64" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M64" s="6" t="s">
+        <v>1096</v>
+      </c>
+      <c r="N64" s="6" t="s">
+        <v>1097</v>
+      </c>
+      <c r="O64" s="6" t="s">
+        <v>1098</v>
+      </c>
+      <c r="P64" s="6" t="s">
+        <v>1099</v>
+      </c>
+      <c r="Q64" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A65" s="6">
+        <v>65</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H65" s="6">
+        <v>1</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J65" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K65" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L65" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M65" s="6" t="s">
+        <v>1103</v>
+      </c>
+      <c r="N65" s="6" t="s">
+        <v>1104</v>
+      </c>
+      <c r="O65" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="P65" s="6" t="s">
+        <v>1106</v>
+      </c>
+      <c r="Q65" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A66" s="6">
+        <v>66</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H66" s="6">
+        <v>1</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K66" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L66" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M66" s="6" t="s">
+        <v>1110</v>
+      </c>
+      <c r="N66" s="6" t="s">
+        <v>1111</v>
+      </c>
+      <c r="O66" s="6" t="s">
+        <v>1112</v>
+      </c>
+      <c r="P66" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="Q66" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A67" s="6">
+        <v>67</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H67" s="6">
+        <v>1</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L67" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M67" s="6" t="s">
+        <v>1117</v>
+      </c>
+      <c r="N67" s="6" t="s">
+        <v>1118</v>
+      </c>
+      <c r="O67" s="6" t="s">
+        <v>1119</v>
+      </c>
+      <c r="P67" s="6" t="s">
+        <v>1120</v>
+      </c>
+      <c r="Q67" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A68" s="6">
+        <v>68</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H68" s="6">
+        <v>1</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J68" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K68" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L68" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M68" s="6" t="s">
+        <v>1124</v>
+      </c>
+      <c r="N68" s="6" t="s">
+        <v>1125</v>
+      </c>
+      <c r="O68" s="6" t="s">
+        <v>1126</v>
+      </c>
+      <c r="P68" s="6" t="s">
+        <v>1127</v>
+      </c>
+      <c r="Q68" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A69" s="6">
+        <v>69</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>1130</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H69" s="6">
+        <v>1</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J69" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K69" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L69" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M69" s="6" t="s">
+        <v>1131</v>
+      </c>
+      <c r="N69" s="6" t="s">
+        <v>1132</v>
+      </c>
+      <c r="O69" s="6" t="s">
+        <v>1133</v>
+      </c>
+      <c r="P69" s="6" t="s">
+        <v>1134</v>
+      </c>
+      <c r="Q69" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A70" s="6">
+        <v>70</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H70" s="6">
+        <v>1</v>
+      </c>
+      <c r="I70" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J70" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K70" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L70" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M70" s="6" t="s">
+        <v>1138</v>
+      </c>
+      <c r="N70" s="6" t="s">
+        <v>1139</v>
+      </c>
+      <c r="O70" s="6" t="s">
+        <v>1140</v>
+      </c>
+      <c r="P70" s="6" t="s">
+        <v>1141</v>
+      </c>
+      <c r="Q70" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A71" s="6">
+        <v>71</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H71" s="6">
+        <v>1</v>
+      </c>
+      <c r="I71" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J71" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L71" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M71" s="6" t="s">
+        <v>1145</v>
+      </c>
+      <c r="N71" s="6" t="s">
+        <v>1146</v>
+      </c>
+      <c r="O71" s="6" t="s">
+        <v>1147</v>
+      </c>
+      <c r="P71" s="6" t="s">
+        <v>1148</v>
+      </c>
+      <c r="Q71" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A72" s="6">
+        <v>72</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H72" s="6">
+        <v>1</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J72" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L72" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M72" s="6" t="s">
+        <v>1152</v>
+      </c>
+      <c r="N72" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="O72" s="6" t="s">
+        <v>1154</v>
+      </c>
+      <c r="P72" s="6" t="s">
+        <v>1155</v>
+      </c>
+      <c r="Q72" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A73" s="6">
+        <v>73</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H73" s="6">
+        <v>1</v>
+      </c>
+      <c r="I73" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J73" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="K73" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L73" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M73" s="6" t="s">
+        <v>1160</v>
+      </c>
+      <c r="N73" s="6" t="s">
+        <v>1161</v>
+      </c>
+      <c r="O73" s="6" t="s">
+        <v>1162</v>
+      </c>
+      <c r="P73" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="Q73" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A74" s="6">
+        <v>74</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>1166</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>1167</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H74" s="6">
+        <v>1</v>
+      </c>
+      <c r="I74" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="K74" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L74" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M74" s="6" t="s">
+        <v>1168</v>
+      </c>
+      <c r="N74" s="6" t="s">
+        <v>1169</v>
+      </c>
+      <c r="O74" s="6" t="s">
+        <v>1170</v>
+      </c>
+      <c r="P74" s="6" t="s">
+        <v>1171</v>
+      </c>
+      <c r="Q74" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A75" s="6">
+        <v>75</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H75" s="6">
+        <v>1</v>
+      </c>
+      <c r="I75" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J75" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="K75" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L75" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M75" s="6" t="s">
+        <v>1176</v>
+      </c>
+      <c r="N75" s="6" t="s">
+        <v>1177</v>
+      </c>
+      <c r="O75" s="6" t="s">
+        <v>1178</v>
+      </c>
+      <c r="P75" s="6" t="s">
+        <v>1179</v>
+      </c>
+      <c r="Q75" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A76" s="6">
+        <v>76</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H76" s="6">
+        <v>1</v>
+      </c>
+      <c r="I76" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J76" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K76" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L76" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M76" s="6" t="s">
+        <v>1183</v>
+      </c>
+      <c r="N76" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="O76" s="6" t="s">
+        <v>1184</v>
+      </c>
+      <c r="P76" s="6" t="s">
+        <v>1185</v>
+      </c>
+      <c r="Q76" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A77" s="6">
+        <v>77</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H77" s="6">
+        <v>1</v>
+      </c>
+      <c r="I77" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J77" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K77" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L77" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M77" s="6" t="s">
+        <v>1189</v>
+      </c>
+      <c r="N77" s="6" t="s">
+        <v>1190</v>
+      </c>
+      <c r="O77" s="6" t="s">
+        <v>1191</v>
+      </c>
+      <c r="P77" s="6" t="s">
+        <v>1192</v>
+      </c>
+      <c r="Q77" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A78" s="6">
+        <v>78</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H78" s="6">
+        <v>1</v>
+      </c>
+      <c r="I78" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K78" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L78" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M78" s="6" t="s">
+        <v>1196</v>
+      </c>
+      <c r="N78" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="O78" s="6" t="s">
+        <v>1197</v>
+      </c>
+      <c r="P78" s="6" t="s">
+        <v>1198</v>
+      </c>
+      <c r="Q78" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A79" s="6">
+        <v>79</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H79" s="6">
+        <v>1</v>
+      </c>
+      <c r="I79" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K79" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L79" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M79" s="6" t="s">
+        <v>1202</v>
+      </c>
+      <c r="N79" s="6" t="s">
+        <v>1203</v>
+      </c>
+      <c r="O79" s="6" t="s">
+        <v>1204</v>
+      </c>
+      <c r="P79" s="6" t="s">
+        <v>1205</v>
+      </c>
+      <c r="Q79" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A80" s="6">
+        <v>80</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>1208</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>1209</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H80" s="6">
+        <v>1</v>
+      </c>
+      <c r="I80" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J80" s="6" t="s">
+        <v>676</v>
+      </c>
+      <c r="K80" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L80" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M80" s="6" t="s">
+        <v>1210</v>
+      </c>
+      <c r="N80" s="6" t="s">
+        <v>1211</v>
+      </c>
+      <c r="O80" s="6" t="s">
+        <v>1212</v>
+      </c>
+      <c r="P80" s="6" t="s">
+        <v>1213</v>
+      </c>
+      <c r="Q80" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A81" s="6">
+        <v>81</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H81" s="6">
+        <v>1</v>
+      </c>
+      <c r="I81" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J81" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K81" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L81" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M81" s="6" t="s">
+        <v>1217</v>
+      </c>
+      <c r="N81" s="6" t="s">
+        <v>1218</v>
+      </c>
+      <c r="O81" s="6" t="s">
+        <v>1219</v>
+      </c>
+      <c r="P81" s="6" t="s">
+        <v>1220</v>
+      </c>
+      <c r="Q81" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A82" s="6">
+        <v>82</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H82" s="6">
+        <v>1</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J82" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K82" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L82" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M82" s="6" t="s">
+        <v>1225</v>
+      </c>
+      <c r="N82" s="6" t="s">
+        <v>1226</v>
+      </c>
+      <c r="O82" s="6" t="s">
+        <v>1227</v>
+      </c>
+      <c r="P82" s="6" t="s">
+        <v>1228</v>
+      </c>
+      <c r="Q82" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A83" s="6">
+        <v>83</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>1231</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>1233</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H83" s="6">
+        <v>1</v>
+      </c>
+      <c r="I83" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J83" s="6" t="s">
+        <v>676</v>
+      </c>
+      <c r="K83" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L83" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M83" s="6" t="s">
+        <v>1234</v>
+      </c>
+      <c r="N83" s="6" t="s">
+        <v>1235</v>
+      </c>
+      <c r="O83" s="6" t="s">
+        <v>1236</v>
+      </c>
+      <c r="P83" s="6" t="s">
+        <v>1237</v>
+      </c>
+      <c r="Q83" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A84" s="6">
+        <v>84</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H84" s="6">
+        <v>1</v>
+      </c>
+      <c r="I84" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J84" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K84" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L84" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M84" s="6" t="s">
+        <v>1241</v>
+      </c>
+      <c r="N84" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="O84" s="6" t="s">
+        <v>1242</v>
+      </c>
+      <c r="P84" s="6" t="s">
+        <v>1243</v>
+      </c>
+      <c r="Q84" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A85" s="6">
+        <v>85</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>1246</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>1247</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H85" s="6">
+        <v>1</v>
+      </c>
+      <c r="I85" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J85" s="6" t="s">
+        <v>676</v>
+      </c>
+      <c r="K85" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L85" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M85" s="6" t="s">
+        <v>1248</v>
+      </c>
+      <c r="N85" s="6" t="s">
+        <v>1249</v>
+      </c>
+      <c r="O85" s="6" t="s">
+        <v>1250</v>
+      </c>
+      <c r="P85" s="6" t="s">
+        <v>1251</v>
+      </c>
+      <c r="Q85" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A86" s="6">
+        <v>86</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>1254</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H86" s="6">
+        <v>1</v>
+      </c>
+      <c r="I86" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J86" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K86" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L86" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M86" s="6" t="s">
+        <v>1256</v>
+      </c>
+      <c r="N86" s="6" t="s">
+        <v>1257</v>
+      </c>
+      <c r="O86" s="6" t="s">
+        <v>1258</v>
+      </c>
+      <c r="P86" s="6" t="s">
+        <v>1259</v>
+      </c>
+      <c r="Q86" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A87" s="6">
+        <v>87</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>1262</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H87" s="6">
+        <v>1</v>
+      </c>
+      <c r="I87" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K87" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L87" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M87" s="6" t="s">
+        <v>1263</v>
+      </c>
+      <c r="N87" s="6" t="s">
+        <v>1264</v>
+      </c>
+      <c r="O87" s="6" t="s">
+        <v>1265</v>
+      </c>
+      <c r="P87" s="6" t="s">
+        <v>1266</v>
+      </c>
+      <c r="Q87" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A88" s="6">
+        <v>88</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>1269</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H88" s="6">
+        <v>1</v>
+      </c>
+      <c r="I88" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J88" s="6" t="s">
+        <v>1017</v>
+      </c>
+      <c r="K88" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L88" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M88" s="6" t="s">
+        <v>1270</v>
+      </c>
+      <c r="N88" s="6" t="s">
+        <v>1271</v>
+      </c>
+      <c r="O88" s="6" t="s">
+        <v>1272</v>
+      </c>
+      <c r="P88" s="6" t="s">
+        <v>1273</v>
+      </c>
+      <c r="Q88" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A89" s="6">
+        <v>89</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>1277</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H89" s="6">
+        <v>1</v>
+      </c>
+      <c r="I89" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J89" s="6" t="s">
+        <v>1017</v>
+      </c>
+      <c r="K89" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L89" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M89" s="6" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N89" s="6" t="s">
+        <v>1279</v>
+      </c>
+      <c r="O89" s="6" t="s">
+        <v>1280</v>
+      </c>
+      <c r="P89" s="6" t="s">
+        <v>1281</v>
+      </c>
+      <c r="Q89" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A90" s="6">
+        <v>90</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G90" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H90" s="6">
+        <v>1</v>
+      </c>
+      <c r="I90" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J90" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K90" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L90" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M90" s="6" t="s">
+        <v>1286</v>
+      </c>
+      <c r="N90" s="6" t="s">
+        <v>1287</v>
+      </c>
+      <c r="O90" s="6" t="s">
+        <v>1288</v>
+      </c>
+      <c r="P90" s="6" t="s">
+        <v>1289</v>
+      </c>
+      <c r="Q90" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A91" s="6">
+        <v>91</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>1292</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G91" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H91" s="6">
+        <v>1</v>
+      </c>
+      <c r="I91" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J91" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="K91" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L91" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M91" s="6" t="s">
+        <v>1294</v>
+      </c>
+      <c r="N91" s="6" t="s">
+        <v>1295</v>
+      </c>
+      <c r="O91" s="6" t="s">
+        <v>1296</v>
+      </c>
+      <c r="P91" s="6" t="s">
+        <v>1297</v>
+      </c>
+      <c r="Q91" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A92" s="6">
+        <v>92</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>1300</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G92" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H92" s="6">
+        <v>1</v>
+      </c>
+      <c r="I92" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J92" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K92" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L92" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M92" s="6" t="s">
+        <v>1301</v>
+      </c>
+      <c r="N92" s="6" t="s">
+        <v>1302</v>
+      </c>
+      <c r="O92" s="6" t="s">
+        <v>1303</v>
+      </c>
+      <c r="P92" s="6" t="s">
+        <v>1304</v>
+      </c>
+      <c r="Q92" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A93" s="6">
+        <v>93</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H93" s="6">
+        <v>1</v>
+      </c>
+      <c r="I93" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J93" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K93" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L93" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M93" s="6" t="s">
+        <v>1308</v>
+      </c>
+      <c r="N93" s="6" t="s">
+        <v>1309</v>
+      </c>
+      <c r="O93" s="6" t="s">
+        <v>1310</v>
+      </c>
+      <c r="P93" s="6" t="s">
+        <v>1311</v>
+      </c>
+      <c r="Q93" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A94" s="6">
+        <v>94</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>1314</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="G94" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H94" s="6">
+        <v>1</v>
+      </c>
+      <c r="I94" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J94" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K94" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L94" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M94" s="6" t="s">
+        <v>1315</v>
+      </c>
+      <c r="N94" s="6" t="s">
+        <v>1316</v>
+      </c>
+      <c r="O94" s="6" t="s">
+        <v>1317</v>
+      </c>
+      <c r="P94" s="6" t="s">
+        <v>1318</v>
+      </c>
+      <c r="Q94" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A95" s="6">
+        <v>95</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>1321</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>1247</v>
+      </c>
+      <c r="G95" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H95" s="6">
+        <v>1</v>
+      </c>
+      <c r="I95" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J95" s="6" t="s">
+        <v>676</v>
+      </c>
+      <c r="K95" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L95" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M95" s="6" t="s">
+        <v>1322</v>
+      </c>
+      <c r="N95" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="O95" s="6" t="s">
+        <v>1323</v>
+      </c>
+      <c r="P95" s="6" t="s">
+        <v>1324</v>
+      </c>
+      <c r="Q95" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A96" s="6">
+        <v>96</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>1327</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>1328</v>
+      </c>
+      <c r="G96" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H96" s="6">
+        <v>1</v>
+      </c>
+      <c r="I96" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J96" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K96" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L96" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M96" s="6" t="s">
+        <v>1329</v>
+      </c>
+      <c r="N96" s="6" t="s">
+        <v>1330</v>
+      </c>
+      <c r="O96" s="6" t="s">
+        <v>1331</v>
+      </c>
+      <c r="P96" s="6" t="s">
+        <v>1332</v>
+      </c>
+      <c r="Q96" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A97" s="6">
+        <v>97</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="E97" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F97" s="6" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G97" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H97" s="6">
+        <v>1</v>
+      </c>
+      <c r="I97" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J97" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K97" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L97" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M97" s="6" t="s">
+        <v>1336</v>
+      </c>
+      <c r="N97" s="6" t="s">
+        <v>1337</v>
+      </c>
+      <c r="O97" s="6" t="s">
+        <v>1338</v>
+      </c>
+      <c r="P97" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="Q97" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A98" s="6">
+        <v>98</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>1342</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>1343</v>
+      </c>
+      <c r="G98" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H98" s="6">
+        <v>1</v>
+      </c>
+      <c r="I98" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J98" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K98" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L98" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M98" s="6" t="s">
+        <v>1344</v>
+      </c>
+      <c r="N98" s="6" t="s">
+        <v>1345</v>
+      </c>
+      <c r="O98" s="6" t="s">
+        <v>1346</v>
+      </c>
+      <c r="P98" s="6" t="s">
+        <v>1347</v>
+      </c>
+      <c r="Q98" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A99" s="6">
+        <v>99</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>1350</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G99" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H99" s="6">
+        <v>1</v>
+      </c>
+      <c r="I99" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J99" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="K99" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L99" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M99" s="6" t="s">
+        <v>1351</v>
+      </c>
+      <c r="N99" s="6" t="s">
+        <v>1352</v>
+      </c>
+      <c r="O99" s="6" t="s">
+        <v>1353</v>
+      </c>
+      <c r="P99" s="6" t="s">
+        <v>1354</v>
+      </c>
+      <c r="Q99" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A100" s="6">
+        <v>100</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>1357</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G100" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="H100" s="6">
+        <v>1</v>
+      </c>
+      <c r="I100" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J100" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="K100" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L100" s="7">
+        <v>45823</v>
+      </c>
+      <c r="M100" s="6" t="s">
+        <v>1359</v>
+      </c>
+      <c r="N100" s="6" t="s">
+        <v>1360</v>
+      </c>
+      <c r="O100" s="6" t="s">
+        <v>1361</v>
+      </c>
+      <c r="P100" s="6" t="s">
+        <v>1362</v>
+      </c>
+      <c r="Q100" s="6" t="s">
         <v>658</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add the test cases 0-99 for limit module
</commit_message>
<xml_diff>
--- a/limits.xlsx
+++ b/limits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed.El-Sawy\Documents\hdb_test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CACC8A-4740-431D-8484-27C905869878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EABC05B-59FE-4CF7-B020-008045CF4FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3D412268-5103-411D-BBE4-3652EEC1385B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2804" uniqueCount="1364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2804" uniqueCount="1384">
   <si>
     <t>Limit</t>
   </si>
@@ -6617,6 +6617,66 @@
     <t>LIM-80</t>
   </si>
   <si>
+    <t>LIM-81</t>
+  </si>
+  <si>
+    <t>LIM-82</t>
+  </si>
+  <si>
+    <t>LIM-83</t>
+  </si>
+  <si>
+    <t>LIM-84</t>
+  </si>
+  <si>
+    <t>LIM-85</t>
+  </si>
+  <si>
+    <t>LIM-86</t>
+  </si>
+  <si>
+    <t>LIM-87</t>
+  </si>
+  <si>
+    <t>LIM-88</t>
+  </si>
+  <si>
+    <t>LIM-89</t>
+  </si>
+  <si>
+    <t>LIM-90</t>
+  </si>
+  <si>
+    <t>LIM-91</t>
+  </si>
+  <si>
+    <t>LIM-92</t>
+  </si>
+  <si>
+    <t>LIM-93</t>
+  </si>
+  <si>
+    <t>LIM-94</t>
+  </si>
+  <si>
+    <t>LIM-95</t>
+  </si>
+  <si>
+    <t>LIM-96</t>
+  </si>
+  <si>
+    <t>LIM-97</t>
+  </si>
+  <si>
+    <t>LIM-98</t>
+  </si>
+  <si>
+    <t>LIM-99</t>
+  </si>
+  <si>
+    <t>LIM-100</t>
+  </si>
+  <si>
     <t xml:space="preserve">	1. Maker logged in 
 2. Limit selected 
 3. Limit cancelled successfully 
@@ -6694,15 +6754,9 @@
     <t>Limit must already exist</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Navigate to LIMIT.INQUIRY &gt; 3. Search for existing overdrawn limit &gt; 4. Review display &gt; 5. Validate language of data &gt; 6. Review format of numbers and dates &gt; 7. Check for unnecessary system messages &gt; 8. Verify all search fields work correctly</t>
-  </si>
-  <si>
     <t>Limit ID: Existing overdrawn</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Inquiry screen accessed &gt; 3. Limit data retrieved &gt; 4. Data displayed clearly &gt; 5. Displayed in original input language &gt; 6. Dates and numbers are correctly formatted &gt; 7. No irrelevant system messages shown &gt; 8. All search filters work properly</t>
-  </si>
-  <si>
     <t>Overdrawn limit retrieved successfully and data shown clearly in original language</t>
   </si>
   <si>
@@ -6712,15 +6766,9 @@
     <t>Inquire all limit codes and verify display in Arabic</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Navigate to LIMIT.INQUIRY &gt; 3. Execute search for all limit codes &gt; 4. Review display</t>
-  </si>
-  <si>
     <t>Search: All codes</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Inquiry screen accessed &gt; 3. Limit codes displayed &gt; 4. All codes and names shown in Arabic</t>
-  </si>
-  <si>
     <t>Display confirmed in Arabic</t>
   </si>
   <si>
@@ -6733,15 +6781,9 @@
     <t>Customer and account must exist</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Open LINK screen &gt; 3. Select target account &gt; 4. Review previously entered data &gt; 5. Click Confirm</t>
-  </si>
-  <si>
     <t>Customer ID and account selected</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. LINK screen opened &gt; 3. Account selected &gt; 4. Data verified &gt; 5. Limit linked to facility successfully</t>
-  </si>
-  <si>
     <t>Limit linked and made available for use</t>
   </si>
   <si>
@@ -6757,15 +6799,9 @@
     <t>LIMIT.CERTIFY</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Open uncertified limits &gt; 3. Select required record &gt; 4. Verify amended fields &gt; 5. Certify the limit</t>
-  </si>
-  <si>
     <t>Amendments include value, authority, duration, guarantees</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Record selected &gt; 3. Data verified &gt; 4. Certification submitted &gt; 5. Limit moved to certified status</t>
-  </si>
-  <si>
     <t>Amended limit successfully certified and now visible in inquiry</t>
   </si>
   <si>
@@ -6778,15 +6814,9 @@
     <t>Limit must be created first</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Open uncertified limits &gt; 3. Select the general limit &gt; 4. Verify sublimits and data &gt; 5. Certify</t>
-  </si>
-  <si>
     <t>Includes: loan sublimit, short term credit sublimit, non-rotating guarantee limit</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. General limit selected &gt; 3. Sublimit data verified &gt; 4. Certification submitted &gt; 5. Limit moved to certified status</t>
-  </si>
-  <si>
     <t>Certification successful, sublimits validated and approved</t>
   </si>
   <si>
@@ -6799,15 +6829,9 @@
     <t>Valid customer and related party numbers</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Open LIMIT.ENTRY screen &gt; 3. Enter valid banking number, limit type, and serial &gt; 4. Input all financial and collateral details &gt; 5. Save the limit record</t>
-  </si>
-  <si>
     <t>Limit Amount: 100,000,000; Currency: EGP; Authority: Branch Manager; Margin: 4%; Interest Rate: 13.5%; Linked Customer: Yes</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Limit screen opened &gt; 3. Data entered successfully &gt; 4. Record saved without error &gt; 5. Limit appears in uncertified limits</t>
-  </si>
-  <si>
     <t>Incomplete or invalid values prevent saving the record</t>
   </si>
   <si>
@@ -6820,15 +6844,9 @@
     <t>Customer and rent assignment documentation ready</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Open LIMIT.ENTRY screen &gt; 3. Enter customer and account info &gt; 4. Input lease-related collateral &gt; 5. Complete and save limit details</t>
-  </si>
-  <si>
     <t>Currency: EGP; Margin: 5%; Interest Rate: 14.5%; Authority: Credit Committee</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Lease data entered correctly &gt; 3. All required limit fields completed &gt; 4. Limit saved and shown in uncertified list &gt; 5. Message confirms contract and promissory note</t>
-  </si>
-  <si>
     <t>Limit successfully created and ready for certification</t>
   </si>
   <si>
@@ -6841,15 +6859,9 @@
     <t>Limit already created and linked</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Open certification screen &gt; 3. Select the linked short-term credit limit &gt; 4. Validate details &gt; 5. Certify and test usage</t>
-  </si>
-  <si>
     <t>Account Branch: Must not be in restricted branch list</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Limit selected &gt; 3. Data confirmed &gt; 4. Certification successful &gt; 5. Warning if usage attempted from restricted branch (e.g., Mohandessin)</t>
-  </si>
-  <si>
     <t>Limit certified but usage must follow branch access rules</t>
   </si>
   <si>
@@ -6862,15 +6874,9 @@
     <t>Amended limit record exists</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Open uncertified limits &gt; 3. Select guarantee limit &gt; 4. Validate updated review cycle and activation date &gt; 5. Certify</t>
-  </si>
-  <si>
     <t>Review Cycle: Changed; Activation Date: Updated</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Limit selected &gt; 3. Changes validated &gt; 4. Certification successful &gt; 5. Limit appears in certified list</t>
-  </si>
-  <si>
     <t>Certification confirms all modified fields are valid</t>
   </si>
   <si>
@@ -6883,15 +6889,9 @@
     <t>Uncertified limit record must exist</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Open uncertified limits &gt; 3. Select general limit &gt; 4. Validate sublimits and branch source &gt; 5. Certify</t>
-  </si>
-  <si>
     <t>Branch: 10th Ramadan; Limit includes short-term credit + loan</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. General limit with sublimits selected &gt; 3. Branch and data validated &gt; 4. Certification completed &gt; 5. Limit visible in certified list</t>
-  </si>
-  <si>
     <t>Limit and all sublimits certified successfully</t>
   </si>
   <si>
@@ -6904,15 +6904,9 @@
     <t>Customer record in 10th Ramadan branch</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Open LIMIT.ENTRY screen &gt; 3. Enter customer info and product code &gt; 4. Input financial values and period &gt; 5. Save record</t>
-  </si>
-  <si>
     <t>Limit Amount: 100,000,000; Interest Rate: 14%; Authority: Branch Manager; Limit Availability: R</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Limit screen opened &gt; 3. Valid data entered &gt; 4. Limit saved successfully &gt; 5. Limit appears in uncertified limits</t>
-  </si>
-  <si>
     <t>Limit is saved and ready for certification</t>
   </si>
   <si>
@@ -6925,15 +6919,9 @@
     <t>Customer has loan and real estate records ready</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Enter loan limit details including customer and purpose &gt; 3. Add real estate collateral info &gt; 4. Link to loan module (EOM3) &gt; 5. Save</t>
-  </si>
-  <si>
     <t>Loan Amount: 1,000,000; Interest Rate: 14.5%; Collateral Value: 6,000,000; Repayment: 2 years</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Loan and collateral data input &gt; 3. Data validated &gt; 4. Limit saved &gt; 5. Appears in uncertified list with proper linkage to loan product</t>
-  </si>
-  <si>
     <t>Loan limit created with all linkages and validations correct</t>
   </si>
   <si>
@@ -6946,15 +6934,9 @@
     <t>Limit must exist in uncertified status</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Select fixed car loan limit &gt; 3. Review loan and installment info &gt; 4. Validate car count and amounts &gt; 5. Certify</t>
-  </si>
-  <si>
     <t>4 cars x 250,000 EGP each; Total: 1,000,000</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Loan details reviewed &gt; 3. Certification confirmed &gt; 4. Certified record appears in system &gt; 5. Loans can be disbursed against limit</t>
-  </si>
-  <si>
     <t>Limit certified and cars can be financed per schedule</t>
   </si>
   <si>
@@ -6967,15 +6949,9 @@
     <t>Uncertified short-term limit available</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Select short-term limit &gt; 3. Verify account details &gt; 4. Certify linkage &gt; 5. Attempt test transaction</t>
-  </si>
-  <si>
     <t>Amount: 100,000; Branch availability: must match</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Limit selected and certified &gt; 3. Test transaction from account performed &gt; 4. Rejection shown if limit not available &gt; 5. System prevents unauthorized usage</t>
-  </si>
-  <si>
     <t>Certification valid, but usage depends on general limit availability</t>
   </si>
   <si>
@@ -6988,15 +6964,9 @@
     <t>Limit must be in uncertified state with modifications</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Open uncertified limits &gt; 3. Select target limit &gt; 4. Confirm variable status and new guarantee details &gt; 5. Certify</t>
-  </si>
-  <si>
     <t>New Guarantee: Increased; Max Value: Specified</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Variable type confirmed &gt; 3. Guarantee reviewed &gt; 4. Certification processed &gt; 5. Certified limit shown in results</t>
-  </si>
-  <si>
     <t>Limit certified with updated variable terms and guarantees</t>
   </si>
   <si>
@@ -7006,15 +6976,9 @@
     <t>Limit record exists in uncertified state</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Select general limit &gt; 3. Confirm inclusion of all sublimits &gt; 4. Certify full limit structure &gt; 5. Verify system update</t>
-  </si>
-  <si>
     <t>Includes: Loan (Car Financing), Short-term credit, Non-rotating guarantee</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. All products included validated &gt; 3. Limit structure certified &gt; 4. System reflects final certified record &gt; 5. No issues raised during save</t>
-  </si>
-  <si>
     <t>All sublimits certified under general limit as expected</t>
   </si>
   <si>
@@ -7027,15 +6991,9 @@
     <t>Customer and debit account exist in system</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Input customer details and debit account &gt; 3. Enter limit values and duration &gt; 4. Confirm no collateral &gt; 5. Save</t>
-  </si>
-  <si>
     <t>Limit Amount: 100,000,000; Interest Rate: 12%; Limit Availability: N</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Data filled in &gt; 3. Limit saved &gt; 4. Appears in uncertified list &gt; 5. Data matches business rules</t>
-  </si>
-  <si>
     <t>Limit successfully created with all conditions met</t>
   </si>
   <si>
@@ -7048,15 +7006,9 @@
     <t>Customer with term deposit account</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Enter customer and deposit info &gt; 3. Define limit as non-rotating guarantee &gt; 4. Input financial data &gt; 5. Save record</t>
-  </si>
-  <si>
     <t>Limit: 250,000; Collateral: 400,000 Deposit; Duration: 1 year</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Guarantee details entered &gt; 3. Deposit linked &gt; 4. Limit saved &gt; 5. Record appears in uncertified list</t>
-  </si>
-  <si>
     <t>Limit saved and linked to deposit guarantee correctly</t>
   </si>
   <si>
@@ -7069,15 +7021,9 @@
     <t>Uncertified modified limit record available</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Select updated limit &gt; 3. Validate new collateral value &gt; 4. Confirm change to variable type &gt; 5. Certify</t>
-  </si>
-  <si>
     <t>Collateral Value: Increased; Limit Type: Changed to variable</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Data reviewed &gt; 3. Certification completed &gt; 4. Record now certified &gt; 5. Appears in search results</t>
-  </si>
-  <si>
     <t>Certification successful with new limit terms</t>
   </si>
   <si>
@@ -7090,24 +7036,15 @@
     <t>Limit record in uncertified list</t>
   </si>
   <si>
-    <t>1. Login as Maker &gt; 2. Select the mortgage limit &gt; 3. Confirm data accuracy &gt; 4. Certify &gt; 5. Ensure limit appears in results</t>
-  </si>
-  <si>
     <t>Limit Type: Mortgage Loan; Status: Non-rotating</t>
   </si>
   <si>
-    <t>1. Maker logged in &gt; 2. Mortgage limit selected &gt; 3. Data validated &gt; 4. Certification saved &gt; 5. Limit appears in certified list</t>
-  </si>
-  <si>
     <t>Limit certified as non-rotating mortgage product</t>
   </si>
   <si>
     <t>limit_document_real_estate_non_revolving_maker</t>
   </si>
   <si>
-    <t>Open the unconfirmed limits screen &gt; Select the limit to be documented &gt; Review the previously entered data &gt; Authorize the limit</t>
-  </si>
-  <si>
     <t>Limit must be previously created and available in unconfirmed state</t>
   </si>
   <si>
@@ -7123,69 +7060,33 @@
     <t>Today</t>
   </si>
   <si>
-    <t>1. Open the unconfirmed limits screen &gt; 2. Select the limit to be documented &gt; 3. Review the previously entered data &gt; 4. Authorize the limit</t>
-  </si>
-  <si>
     <t>No inputs needed – system retrieves existing data</t>
   </si>
   <si>
-    <t>1. System shows the selected limit &gt; 2. Data review allowed &gt; 3. User authorizes the limit &gt; 4. Limit moves to the confirmed state and appears in inquiry</t>
-  </si>
-  <si>
     <t>limit_create_real_estate_non_rotating_without_guarantee_maker</t>
   </si>
   <si>
-    <t>Create new limit for individual customer &gt; Use valid CIF and debit account &gt; Fill all required dates in proper order &gt; Set limit amount to 750,000 EGP &gt; Disburse in 3 equal tranches &gt; Save</t>
-  </si>
-  <si>
     <t>CIF, debit account, pricing info ready</t>
   </si>
   <si>
-    <t>1. Login as maker &gt; 2. Navigate to Limit creation screen &gt; 3. Enter individual CIF and debit account &gt; 4. Set type as non-revolving without guarantee &gt; 5. Set amount: 750,000 EGP &gt; 6. Set duration: 1 year &gt; 7. Set tranche details (3 equal) &gt; 8. Fill all required dates in sequence &gt; 9. Save the limit</t>
-  </si>
-  <si>
     <t>Customer: Individual; Currency: EGP; Amount: 750,000; Authority: Branch Manager; Disbursement: 3 equal tranches; Duration: 1 year</t>
   </si>
   <si>
-    <t>1. Limit screen opens &gt; 2. Data accepted &gt; 3. Limit saved in unconfirmed limits &gt; 4. Appears under unconfirmed list for documentation</t>
-  </si>
-  <si>
     <t>limit_create_general_non_rotating_with_pledge_company_maker</t>
   </si>
   <si>
-    <t>Create a non-revolving limit for a company customer with pledge guarantee of 750,000 EGP &gt; Set all required fields and dates &gt; Save</t>
-  </si>
-  <si>
     <t>CIF (Company), debit account, pledge details</t>
   </si>
   <si>
-    <t>1. Login as maker &gt; 2. Open Limit creation screen &gt; 3. Enter valid company CIF &gt; 4. Enter type as general non-revolving &gt; 5. Enter amount: 750,000 EGP &gt; 6. Select guarantee type: commercial pledge &gt; 7. Set all relevant dates &gt; 8. Save the limit</t>
-  </si>
-  <si>
     <t>Currency: EGP; Amount: 750,000; Guarantee: Pledge; Duration: 1 year; Authority: Regional level</t>
   </si>
   <si>
-    <t>1. Limit screen opens &gt; 2. Data is saved correctly &gt; 3. Message confirms contract and promissory note &gt; 4. Limit saved under unconfirmed limits</t>
-  </si>
-  <si>
     <t>limit_document_short_term_facility_linked_to_collected_documents_maker</t>
   </si>
   <si>
-    <t>Document a short-term facility linked to collected commercial papers &gt; Link account &gt; Review data &gt; Document &gt; Perform test transactions to verify revolving nature</t>
-  </si>
-  <si>
     <t>Limit and account must be created and ready</t>
   </si>
   <si>
-    <t>1. Login as maker &gt; 2. Open "Link limit to account" screen &gt; 3. Select customer’s facility account &gt; 4. Review data &gt; 5. Document the linkage &gt; 6. Perform debit transaction: 35,000 EGP &gt; 7. Perform credit transaction after 2 days: 12,000 EGP &gt; 8. Another credit after a week: 10,000 EGP</t>
-  </si>
-  <si>
-    <t>Account: Customer facility account &gt; Limit Type: Revolving</t>
-  </si>
-  <si>
-    <t>1. Limit linked to account &gt; 2. Usage allowed &gt; 3. Transactions post correctly &gt; 4. Revolving nature verified by multiple debit/credit cycles</t>
-  </si>
-  <si>
     <t>limit_document_limit_with_modified_dates_and_notes_maker</t>
   </si>
   <si>
@@ -7195,15 +7096,9 @@
     <t>Limit must be modified prior to documentation</t>
   </si>
   <si>
-    <t>1. Open unconfirmed limits screen &gt; 2. Select modified limit &gt; 3. Review changes &gt; 4. Authorize the limit</t>
-  </si>
-  <si>
     <t>No new input required – already modified</t>
   </si>
   <si>
-    <t>1. Modified limit is visible &gt; 2. Changes appear correctly &gt; 3. Limit is authorized &gt; 4. Limit appears in confirmed limits inquiry</t>
-  </si>
-  <si>
     <t>limit_document_mixed_limit_types_under_general_limit_maker</t>
   </si>
   <si>
@@ -7213,51 +7108,27 @@
     <t>Mixed type limit must be created first</t>
   </si>
   <si>
-    <t>1. Open unconfirmed limits screen &gt; 2. Select the mixed limit &gt; 3. Review details &gt; 4. Authorize</t>
-  </si>
-  <si>
     <t>Existing mixed limit with all subtypes defined</t>
   </si>
   <si>
-    <t>1. All sub-limit types appear &gt; 2. User confirms details &gt; 3. Limit is documented successfully &gt; 4. Appears under confirmed limits</t>
-  </si>
-  <si>
     <t>limit_add_commercial_paper_guarantee_modify_authority_and_first_disbursal_flag_maker</t>
   </si>
   <si>
-    <t>Add commercial paper guarantee of 190 million EGP to general limit &gt; Change authority to Executive Committee &gt; Set First Disbursal flag to N</t>
-  </si>
-  <si>
     <t>Existing general limit must be created</t>
   </si>
   <si>
-    <t>1. Open Limit creation screen &gt; 2. Modify authority &gt; 3. Add guarantee (Commercial Papers = 190M) &gt; 4. Update First Disbursal to N &gt; 5. Save changes</t>
-  </si>
-  <si>
     <t>Currency: EGP; Guarantee: Commercial Papers; Authority: Executive Committee</t>
   </si>
   <si>
-    <t>1. Modifications saved &gt; 2. Changes appear in modified unconfirmed limits &gt; 3. Once documented, changes appear in confirmed limit inquiry &gt; 4. Guarantee update reflected in guarantee module</t>
-  </si>
-  <si>
     <t>limit_create_general_revolving_company_in_dirham_maker</t>
   </si>
   <si>
-    <t>Create a revolving general limit for a company in AED for 100 million &gt; Set proper dates and authority</t>
-  </si>
-  <si>
     <t>Company CIF, Dirham account, pricing info ready</t>
   </si>
   <si>
-    <t>1. Login as maker &gt; 2. Open limit creation screen &gt; 3. Input company CIF &gt; 4. Set type: General Revolving &gt; 5. Amount: 100 million AED &gt; 6. Fill all required dates &gt; 7. Save</t>
-  </si>
-  <si>
     <t>Amount: 100M AED; Authority: Branch Manager; First Grant: Yes</t>
   </si>
   <si>
-    <t>1. System opens limit screen &gt; 2. Data accepted &gt; 3. Limit saved successfully &gt; 4. Appears in unconfirmed limits list</t>
-  </si>
-  <si>
     <t>limit_document_non_revolving_limit_with_LG_and_LC_sub_limits_maker</t>
   </si>
   <si>
@@ -7267,69 +7138,36 @@
     <t>Limit must include defined sub-limits</t>
   </si>
   <si>
-    <t>1. Open unconfirmed limits screen &gt; 2. Select the non-revolving limit &gt; 3. Review all sub-limits &gt; 4. Authorize the limit</t>
-  </si>
-  <si>
     <t>Limit includes LG and LC types</t>
   </si>
   <si>
-    <t>1. Limit displays all required subtypes &gt; 2. Authorization proceeds &gt; 3. Appears in confirmed limits inquiry</t>
-  </si>
-  <si>
     <t>limit_create_non_revolving_company_with_commercial_paper_pledge_100M_maker</t>
   </si>
   <si>
-    <t>Create general non-revolving limit for company for 100M EGP &gt; Backed by 200M EGP commercial paper &gt; Duration: 1 year</t>
-  </si>
-  <si>
     <t>CIF (Company), pledge, account, rates</t>
   </si>
   <si>
-    <t>1. Login as maker &gt; 2. Enter CIF and account &gt; 3. Set type as non-revolving &gt; 4. Set amount: 100M &gt; 5. Select guarantee: commercial paper &gt; 6. Set all dates &gt; 7. Save</t>
-  </si>
-  <si>
     <t>Amount: 100M EGP; Guarantee: Commercial Paper 200M; Duration: 1 year</t>
   </si>
   <si>
-    <t>1. Limit created successfully &gt; 2. Message confirms contract and promissory note &gt; 3. Limit appears in unconfirmed limits</t>
-  </si>
-  <si>
     <t>limit_create_rotating_facility_in_foreign_currency_company_maker</t>
   </si>
   <si>
-    <t>Create a revolving facility for a company customer in USD &gt; Set amount to 1,000,000 USD &gt; Link to appropriate account &gt; Fill required dates &gt; Save</t>
-  </si>
-  <si>
     <t>Company CIF, USD account, valid rate plan</t>
   </si>
   <si>
-    <t>1. Login as maker &gt; 2. Open Limit creation screen &gt; 3. Enter company CIF &gt; 4. Select type: Revolving &gt; 5. Currency: USD &gt; 6. Amount: 1,000,000 &gt; 7. Link facility account &gt; 8. Set valid dates &gt; 9. Save</t>
-  </si>
-  <si>
     <t>Customer Type: Company; Amount: 1,000,000 USD; Facility Type: Revolving</t>
   </si>
   <si>
-    <t>1. Limit entry accepted &gt; 2. Saved under unconfirmed limits &gt; 3. Visible for documentation step</t>
-  </si>
-  <si>
     <t>limit_create_general_revolving_personal_customer_in_euro_maker</t>
   </si>
   <si>
-    <t>Create a general revolving limit for individual in EUR &gt; Amount: 50,000 EUR &gt; No guarantee &gt; 1-year duration &gt; Save</t>
-  </si>
-  <si>
     <t>CIF, EUR account, personal customer segment</t>
   </si>
   <si>
-    <t>1. Login as maker &gt; 2. Navigate to Limit creation screen &gt; 3. Enter individual CIF &gt; 4. Select type: General Revolving &gt; 5. Currency: EUR &gt; 6. Amount: 50,000 &gt; 7. Duration: 1 year &gt; 8. Save</t>
-  </si>
-  <si>
     <t>Currency: EUR; Amount: 50,000; Duration: 1 year</t>
   </si>
   <si>
-    <t>1. Limit created successfully &gt; 2. Appears in unconfirmed list &gt; 3. Ready for documentation step</t>
-  </si>
-  <si>
     <t>limit_document_with_change_in_currency_and_amount_maker</t>
   </si>
   <si>
@@ -7339,102 +7177,48 @@
     <t>Limit must be modified before documentation</t>
   </si>
   <si>
-    <t>1. Open unconfirmed limits screen &gt; 2. Select modified limit &gt; 3. Review currency and amount changes &gt; 4. Authorize</t>
-  </si>
-  <si>
     <t>Changed from EGP to USD; Amount: 2,000,000</t>
   </si>
   <si>
-    <t>1. Modified limit displayed &gt; 2. Currency and amount reflected correctly &gt; 3. Authorization successful &gt; 4. Appears in confirmed inquiry</t>
-  </si>
-  <si>
     <t>limit_create_short_term_personal_limit_with_guarantee_maker</t>
   </si>
   <si>
-    <t>Create a short-term personal limit with guarantee &gt; Amount: 20,000 EGP &gt; Guarantee: salary transfer &gt; Duration: 6 months</t>
-  </si>
-  <si>
     <t>CIF, salary transfer letter, personal account</t>
   </si>
   <si>
-    <t>1. Login as maker &gt; 2. Navigate to Limit creation screen &gt; 3. Enter individual CIF &gt; 4. Select type: Short-Term &gt; 5. Amount: 20,000 EGP &gt; 6. Select guarantee: Salary transfer &gt; 7. Set duration: 6 months &gt; 8. Save</t>
-  </si>
-  <si>
     <t>Currency: EGP; Guarantee: Salary transfer; Duration: 6 months</t>
   </si>
   <si>
-    <t>1. Limit saved correctly &gt; 2. Appears in unconfirmed limits list &gt; 3. Awaiting documentation</t>
-  </si>
-  <si>
     <t>limit_document_multiple_sub_limits_in_different_currencies_maker</t>
   </si>
   <si>
-    <t>Document a general limit with three sub-limits in EGP, USD, and EUR &gt; Validate all entries &gt; Authorize</t>
-  </si>
-  <si>
     <t>Multi-currency sub-limits must be pre-created</t>
   </si>
   <si>
-    <t>1. Open unconfirmed limits screen &gt; 2. Select limit with sub-limits &gt; 3. Verify sub-limit details &gt; 4. Authorize</t>
-  </si>
-  <si>
     <t>Sub-limits: EGP, USD, EUR; All correct values entered</t>
   </si>
   <si>
-    <t>1. All sub-limits displayed correctly &gt; 2. Authorization proceeds &gt; 3. Limit documented successfully &gt; 4. Visible in confirmed inquiry</t>
-  </si>
-  <si>
     <t>limit_create_term_loan_facility_backed_by_deposit_pledge_maker</t>
   </si>
   <si>
-    <t>Create a term loan limit backed by pledge on time deposit &gt; Amount: 500,000 EGP &gt; Duration: 2 years</t>
-  </si>
-  <si>
     <t>Deposit pledge contract and CIF must exist</t>
   </si>
   <si>
-    <t>1. Login as maker &gt; 2. Create new limit &gt; 3. Set type: Term Loan &gt; 4. Amount: 500,000 EGP &gt; 5. Duration: 2 years &gt; 6. Guarantee: Time Deposit pledge &gt; 7. Save</t>
-  </si>
-  <si>
-    <t>Amount: 500,000; Pledge Type: Deposit &gt; Duration: 2 years</t>
-  </si>
-  <si>
-    <t>1. Limit creation successful &gt; 2. Guarantee reflected &gt; 3. Awaiting documentation</t>
-  </si>
-  <si>
-    <t>limit_document_rejected_limit_after_modification_maker Attempt to document a previously rejected limit after corrections to amount and duration &gt; Validate all fields &gt; Authorize again</t>
-  </si>
-  <si>
     <t>Rejected limit must have been corrected</t>
   </si>
   <si>
-    <t>1. Open rejected limits list &gt; 2. Select corrected limit &gt; 3. Verify all updated fields &gt; 4. Authorize</t>
-  </si>
-  <si>
     <t>Previous rejection resolved (amount/duration corrected)</t>
   </si>
   <si>
-    <t>1. Limit reflects corrected data &gt; 2. Authorization completes &gt; 3. Limit moves to confirmed state</t>
-  </si>
-  <si>
     <t>limit_create_LG_non_rotating_with_maximum_exposure_flag_maker</t>
   </si>
   <si>
-    <t>Create a non-revolving LG limit &gt; Amount: 2M EGP &gt; Flag maximum exposure as active &gt; No additional guarantee</t>
-  </si>
-  <si>
     <t>CIF, account, and LG module active</t>
   </si>
   <si>
-    <t>1. Login as maker &gt; 2. Enter limit screen &gt; 3. Set type: Non-revolving LG &gt; 4. Amount: 2,000,000 EGP &gt; 5. Set Max Exposure = Yes &gt; 6. Save</t>
-  </si>
-  <si>
     <t>Currency: EGP; Type: LG; Exposure Flag: Y</t>
   </si>
   <si>
-    <t>1. Limit saved successfully &gt; 2. Max exposure flag set correctly &gt; 3. Limit shows in unconfirmed list</t>
-  </si>
-  <si>
     <t>limit_document_modification_change_in_guarantee_type_maker</t>
   </si>
   <si>
@@ -7444,38 +7228,671 @@
     <t>Limit must be updated before documentation</t>
   </si>
   <si>
-    <t>1. Open unconfirmed limits &gt; 2. Select modified limit &gt; 3. Verify guarantee type changed &gt; 4. Authorize</t>
-  </si>
-  <si>
-    <t>Old: Pledge &gt; New: Corporate Guarantee</t>
-  </si>
-  <si>
-    <t>1. Guarantee type updated &gt; 2. Documentation proceeds &gt; 3. Limit appears in confirmed list</t>
-  </si>
-  <si>
     <t>limit_create_general_limit_with_special_pricing_table_maker</t>
   </si>
   <si>
-    <t>Create general limit with reference to a special pricing table for interest calculation &gt; Save</t>
-  </si>
-  <si>
     <t>CIF and pricing table must exist in system</t>
   </si>
   <si>
-    <t>1. Login as maker &gt; 2. Access limit creation screen &gt; 3. Input customer CIF &gt; 4. Set limit type: General &gt; 5. Link pricing table: PRICING_2025 &gt; 6. Save</t>
-  </si>
-  <si>
     <t>Currency: EGP; Pricing Table: PRICING_2025</t>
   </si>
   <si>
-    <t>1. Limit saved with correct pricing &gt; 2. Pricing info reflected in inquiry &gt; 3. Limit visible in unconfirmed list</t>
+    <t>1. Login as Maker 
+ 2. Navigate to LIMIT.INQUIRY 
+ 3. Search for existing overdrawn limit 
+ 4. Review display 
+ 5. Validate language of data 
+ 6. Review format of numbers and dates 
+ 7. Check for unnecessary system messages 
+ 8. Verify all search fields work correctly</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Inquiry screen accessed 
+ 3. Limit data retrieved 
+ 4. Data displayed clearly 
+ 5. Displayed in original input language 
+ 6. Dates and numbers are correctly formatted 
+ 7. No irrelevant system messages shown 
+ 8. All search filters work properly</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Navigate to LIMIT.INQUIRY 
+ 3. Execute search for all limit codes 
+ 4. Review display</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Inquiry screen accessed 
+ 3. Limit codes displayed 
+ 4. All codes and names shown in Arabic</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Open LINK screen 
+ 3. Select target account 
+ 4. Review previously entered data 
+ 5. Click Confirm</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. LINK screen opened 
+ 3. Account selected 
+ 4. Data verified 
+ 5. Limit linked to facility successfully</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Open uncertified limits 
+ 3. Select required record 
+ 4. Verify amended fields 
+ 5. Certify the limit</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Record selected 
+ 3. Data verified 
+ 4. Certification submitted 
+ 5. Limit moved to certified status</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Open uncertified limits 
+ 3. Select the general limit 
+ 4. Verify sublimits and data 
+ 5. Certify</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. General limit selected 
+ 3. Sublimit data verified 
+ 4. Certification submitted 
+ 5. Limit moved to certified status</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Open LIMIT.ENTRY screen 
+ 3. Enter valid banking number, limit type, and serial 
+ 4. Input all financial and collateral details 
+ 5. Save the limit record</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Limit screen opened 
+ 3. Data entered successfully 
+ 4. Record saved without error 
+ 5. Limit appears in uncertified limits</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Open LIMIT.ENTRY screen 
+ 3. Enter customer and account info 
+ 4. Input lease-related collateral 
+ 5. Complete and save limit details</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Lease data entered correctly 
+ 3. All required limit fields completed 
+ 4. Limit saved and shown in uncertified list 
+ 5. Message confirms contract and promissory note</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Open certification screen 
+ 3. Select the linked short-term credit limit 
+ 4. Validate details 
+ 5. Certify and test usage</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Limit selected 
+ 3. Data confirmed 
+ 4. Certification successful 
+ 5. Warning if usage attempted from restricted branch (e.g., Mohandessin)</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Open uncertified limits 
+ 3. Select guarantee limit 
+ 4. Validate updated review cycle and activation date 
+ 5. Certify</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Limit selected 
+ 3. Changes validated 
+ 4. Certification successful 
+ 5. Limit appears in certified list</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Open uncertified limits 
+ 3. Select general limit 
+ 4. Validate sublimits and branch source 
+ 5. Certify</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. General limit with sublimits selected 
+ 3. Branch and data validated 
+ 4. Certification completed 
+ 5. Limit visible in certified list</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Open LIMIT.ENTRY screen 
+ 3. Enter customer info and product code 
+ 4. Input financial values and period 
+ 5. Save record</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Limit screen opened 
+ 3. Valid data entered 
+ 4. Limit saved successfully 
+ 5. Limit appears in uncertified limits</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Enter loan limit details including customer and purpose 
+ 3. Add real estate collateral info 
+ 4. Link to loan module (EOM3) 
+ 5. Save</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Loan and collateral data input 
+ 3. Data validated 
+ 4. Limit saved 
+ 5. Appears in uncertified list with proper linkage to loan product</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Select fixed car loan limit 
+ 3. Review loan and installment info 
+ 4. Validate car count and amounts 
+ 5. Certify</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Loan details reviewed 
+ 3. Certification confirmed 
+ 4. Certified record appears in system 
+ 5. Loans can be disbursed against limit</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Select short-term limit 
+ 3. Verify account details 
+ 4. Certify linkage 
+ 5. Attempt test transaction</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Limit selected and certified 
+ 3. Test transaction from account performed 
+ 4. Rejection shown if limit not available 
+ 5. System prevents unauthorized usage</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Open uncertified limits 
+ 3. Select target limit 
+ 4. Confirm variable status and new guarantee details 
+ 5. Certify</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Variable type confirmed 
+ 3. Guarantee reviewed 
+ 4. Certification processed 
+ 5. Certified limit shown in results</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Select general limit 
+ 3. Confirm inclusion of all sublimits 
+ 4. Certify full limit structure 
+ 5. Verify system update</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. All products included validated 
+ 3. Limit structure certified 
+ 4. System reflects final certified record 
+ 5. No issues raised during save</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Input customer details and debit account 
+ 3. Enter limit values and duration 
+ 4. Confirm no collateral 
+ 5. Save</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Data filled in 
+ 3. Limit saved 
+ 4. Appears in uncertified list 
+ 5. Data matches business rules</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Enter customer and deposit info 
+ 3. Define limit as non-rotating guarantee 
+ 4. Input financial data 
+ 5. Save record</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Guarantee details entered 
+ 3. Deposit linked 
+ 4. Limit saved 
+ 5. Record appears in uncertified list</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Select updated limit 
+ 3. Validate new collateral value 
+ 4. Confirm change to variable type 
+ 5. Certify</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Data reviewed 
+ 3. Certification completed 
+ 4. Record now certified 
+ 5. Appears in search results</t>
+  </si>
+  <si>
+    <t>1. Login as Maker 
+ 2. Select the mortgage limit 
+ 3. Confirm data accuracy 
+ 4. Certify 
+ 5. Ensure limit appears in results</t>
+  </si>
+  <si>
+    <t>1. Maker logged in 
+ 2. Mortgage limit selected 
+ 3. Data validated 
+ 4. Certification saved 
+ 5. Limit appears in certified list</t>
+  </si>
+  <si>
+    <t>Open the unconfirmed limits screen 
+ Select the limit to be documented 
+ Review the previously entered data 
+ Authorize the limit</t>
+  </si>
+  <si>
+    <t>1. Open the unconfirmed limits screen 
+ 2. Select the limit to be documented 
+ 3. Review the previously entered data 
+ 4. Authorize the limit</t>
+  </si>
+  <si>
+    <t>1. System shows the selected limit 
+ 2. Data review allowed 
+ 3. User authorizes the limit 
+ 4. Limit moves to the confirmed state and appears in inquiry</t>
+  </si>
+  <si>
+    <t>Create new limit for individual customer 
+ Use valid CIF and debit account 
+ Fill all required dates in proper order 
+ Set limit amount to 750,000 EGP 
+ Disburse in 3 equal tranches 
+ Save</t>
+  </si>
+  <si>
+    <t>1. Login as maker 
+ 2. Navigate to Limit creation screen 
+ 3. Enter individual CIF and debit account 
+ 4. Set type as non-revolving without guarantee 
+ 5. Set amount: 750,000 EGP 
+ 6. Set duration: 1 year 
+ 7. Set tranche details (3 equal) 
+ 8. Fill all required dates in sequence 
+ 9. Save the limit</t>
+  </si>
+  <si>
+    <t>1. Limit screen opens 
+ 2. Data accepted 
+ 3. Limit saved in unconfirmed limits 
+ 4. Appears under unconfirmed list for documentation</t>
+  </si>
+  <si>
+    <t>Create a non-revolving limit for a company customer with pledge guarantee of 750,000 EGP 
+ Set all required fields and dates 
+ Save</t>
+  </si>
+  <si>
+    <t>1. Login as maker 
+ 2. Open Limit creation screen 
+ 3. Enter valid company CIF 
+ 4. Enter type as general non-revolving 
+ 5. Enter amount: 750,000 EGP 
+ 6. Select guarantee type: commercial pledge 
+ 7. Set all relevant dates 
+ 8. Save the limit</t>
+  </si>
+  <si>
+    <t>1. Limit screen opens 
+ 2. Data is saved correctly 
+ 3. Message confirms contract and promissory note 
+ 4. Limit saved under unconfirmed limits</t>
+  </si>
+  <si>
+    <t>Document a short-term facility linked to collected commercial papers 
+ Link account 
+ Review data 
+ Document 
+ Perform test transactions to verify revolving nature</t>
+  </si>
+  <si>
+    <t>1. Login as maker 
+ 2. Open "Link limit to account" screen 
+ 3. Select customer’s facility account 
+ 4. Review data 
+ 5. Document the linkage 
+ 6. Perform debit transaction: 35,000 EGP 
+ 7. Perform credit transaction after 2 days: 12,000 EGP 
+ 8. Another credit after a week: 10,000 EGP</t>
+  </si>
+  <si>
+    <t>Account: Customer facility account 
+ Limit Type: Revolving</t>
+  </si>
+  <si>
+    <t>1. Limit linked to account 
+ 2. Usage allowed 
+ 3. Transactions post correctly 
+ 4. Revolving nature verified by multiple debit/credit cycles</t>
+  </si>
+  <si>
+    <t>1. Open unconfirmed limits screen 
+ 2. Select modified limit 
+ 3. Review changes 
+ 4. Authorize the limit</t>
+  </si>
+  <si>
+    <t>1. Modified limit is visible 
+ 2. Changes appear correctly 
+ 3. Limit is authorized 
+ 4. Limit appears in confirmed limits inquiry</t>
+  </si>
+  <si>
+    <t>1. Open unconfirmed limits screen 
+ 2. Select the mixed limit 
+ 3. Review details 
+ 4. Authorize</t>
+  </si>
+  <si>
+    <t>1. All sub-limit types appear 
+ 2. User confirms details 
+ 3. Limit is documented successfully 
+ 4. Appears under confirmed limits</t>
+  </si>
+  <si>
+    <t>Add commercial paper guarantee of 190 million EGP to general limit 
+ Change authority to Executive Committee 
+ Set First Disbursal flag to N</t>
+  </si>
+  <si>
+    <t>1. Open Limit creation screen 
+ 2. Modify authority 
+ 3. Add guarantee (Commercial Papers = 190M) 
+ 4. Update First Disbursal to N 
+ 5. Save changes</t>
+  </si>
+  <si>
+    <t>1. Modifications saved 
+ 2. Changes appear in modified unconfirmed limits 
+ 3. Once documented, changes appear in confirmed limit inquiry 
+ 4. Guarantee update reflected in guarantee module</t>
+  </si>
+  <si>
+    <t>Create a revolving general limit for a company in AED for 100 million 
+ Set proper dates and authority</t>
+  </si>
+  <si>
+    <t>1. Login as maker 
+ 2. Open limit creation screen 
+ 3. Input company CIF 
+ 4. Set type: General Revolving 
+ 5. Amount: 100 million AED 
+ 6. Fill all required dates 
+ 7. Save</t>
+  </si>
+  <si>
+    <t>1. System opens limit screen 
+ 2. Data accepted 
+ 3. Limit saved successfully 
+ 4. Appears in unconfirmed limits list</t>
+  </si>
+  <si>
+    <t>1. Open unconfirmed limits screen 
+ 2. Select the non-revolving limit 
+ 3. Review all sub-limits 
+ 4. Authorize the limit</t>
+  </si>
+  <si>
+    <t>1. Limit displays all required subtypes 
+ 2. Authorization proceeds 
+ 3. Appears in confirmed limits inquiry</t>
+  </si>
+  <si>
+    <t>Create general non-revolving limit for company for 100M EGP 
+ Backed by 200M EGP commercial paper 
+ Duration: 1 year</t>
+  </si>
+  <si>
+    <t>1. Login as maker 
+ 2. Enter CIF and account 
+ 3. Set type as non-revolving 
+ 4. Set amount: 100M 
+ 5. Select guarantee: commercial paper 
+ 6. Set all dates 
+ 7. Save</t>
+  </si>
+  <si>
+    <t>1. Limit created successfully 
+ 2. Message confirms contract and promissory note 
+ 3. Limit appears in unconfirmed limits</t>
+  </si>
+  <si>
+    <t>Create a revolving facility for a company customer in USD 
+ Set amount to 1,000,000 USD 
+ Link to appropriate account 
+ Fill required dates 
+ Save</t>
+  </si>
+  <si>
+    <t>1. Login as maker 
+ 2. Open Limit creation screen 
+ 3. Enter company CIF 
+ 4. Select type: Revolving 
+ 5. Currency: USD 
+ 6. Amount: 1,000,000 
+ 7. Link facility account 
+ 8. Set valid dates 
+ 9. Save</t>
+  </si>
+  <si>
+    <t>1. Limit entry accepted 
+ 2. Saved under unconfirmed limits 
+ 3. Visible for documentation step</t>
+  </si>
+  <si>
+    <t>Create a general revolving limit for individual in EUR 
+ Amount: 50,000 EUR 
+ No guarantee 
+ 1-year duration 
+ Save</t>
+  </si>
+  <si>
+    <t>1. Login as maker 
+ 2. Navigate to Limit creation screen 
+ 3. Enter individual CIF 
+ 4. Select type: General Revolving 
+ 5. Currency: EUR 
+ 6. Amount: 50,000 
+ 7. Duration: 1 year 
+ 8. Save</t>
+  </si>
+  <si>
+    <t>1. Limit created successfully 
+ 2. Appears in unconfirmed list 
+ 3. Ready for documentation step</t>
+  </si>
+  <si>
+    <t>1. Open unconfirmed limits screen 
+ 2. Select modified limit 
+ 3. Review currency and amount changes 
+ 4. Authorize</t>
+  </si>
+  <si>
+    <t>1. Modified limit displayed 
+ 2. Currency and amount reflected correctly 
+ 3. Authorization successful 
+ 4. Appears in confirmed inquiry</t>
+  </si>
+  <si>
+    <t>Create a short-term personal limit with guarantee 
+ Amount: 20,000 EGP 
+ Guarantee: salary transfer 
+ Duration: 6 months</t>
+  </si>
+  <si>
+    <t>1. Login as maker 
+ 2. Navigate to Limit creation screen 
+ 3. Enter individual CIF 
+ 4. Select type: Short-Term 
+ 5. Amount: 20,000 EGP 
+ 6. Select guarantee: Salary transfer 
+ 7. Set duration: 6 months 
+ 8. Save</t>
+  </si>
+  <si>
+    <t>1. Limit saved correctly 
+ 2. Appears in unconfirmed limits list 
+ 3. Awaiting documentation</t>
+  </si>
+  <si>
+    <t>Document a general limit with three sub-limits in EGP, USD, and EUR 
+ Validate all entries 
+ Authorize</t>
+  </si>
+  <si>
+    <t>1. Open unconfirmed limits screen 
+ 2. Select limit with sub-limits 
+ 3. Verify sub-limit details 
+ 4. Authorize</t>
+  </si>
+  <si>
+    <t>1. All sub-limits displayed correctly 
+ 2. Authorization proceeds 
+ 3. Limit documented successfully 
+ 4. Visible in confirmed inquiry</t>
+  </si>
+  <si>
+    <t>Create a term loan limit backed by pledge on time deposit 
+ Amount: 500,000 EGP 
+ Duration: 2 years</t>
+  </si>
+  <si>
+    <t>1. Login as maker 
+ 2. Create new limit 
+ 3. Set type: Term Loan 
+ 4. Amount: 500,000 EGP 
+ 5. Duration: 2 years 
+ 6. Guarantee: Time Deposit pledge 
+ 7. Save</t>
+  </si>
+  <si>
+    <t>Amount: 500,000; Pledge Type: Deposit 
+ Duration: 2 years</t>
+  </si>
+  <si>
+    <t>1. Limit creation successful 
+ 2. Guarantee reflected 
+ 3. Awaiting documentation</t>
+  </si>
+  <si>
+    <t>limit_document_rejected_limit_after_modification_maker Attempt to document a previously rejected limit after corrections to amount and duration 
+ Validate all fields 
+ Authorize again</t>
+  </si>
+  <si>
+    <t>1. Open rejected limits list 
+ 2. Select corrected limit 
+ 3. Verify all updated fields 
+ 4. Authorize</t>
+  </si>
+  <si>
+    <t>1. Limit reflects corrected data 
+ 2. Authorization completes 
+ 3. Limit moves to confirmed state</t>
+  </si>
+  <si>
+    <t>Create a non-revolving LG limit 
+ Amount: 2M EGP 
+ Flag maximum exposure as active 
+ No additional guarantee</t>
+  </si>
+  <si>
+    <t>1. Login as maker 
+ 2. Enter limit screen 
+ 3. Set type: Non-revolving LG 
+ 4. Amount: 2,000,000 EGP 
+ 5. Set Max Exposure = Yes 
+ 6. Save</t>
+  </si>
+  <si>
+    <t>1. Limit saved successfully 
+ 2. Max exposure flag set correctly 
+ 3. Limit shows in unconfirmed list</t>
+  </si>
+  <si>
+    <t>1. Open unconfirmed limits 
+ 2. Select modified limit 
+ 3. Verify guarantee type changed 
+ 4. Authorize</t>
+  </si>
+  <si>
+    <t>Old: Pledge 
+ New: Corporate Guarantee</t>
+  </si>
+  <si>
+    <t>1. Guarantee type updated 
+ 2. Documentation proceeds 
+ 3. Limit appears in confirmed list</t>
+  </si>
+  <si>
+    <t>Create general limit with reference to a special pricing table for interest calculation 
+ Save</t>
+  </si>
+  <si>
+    <t>1. Login as maker 
+ 2. Access limit creation screen 
+ 3. Input customer CIF 
+ 4. Set limit type: General 
+ 5. Link pricing table: PRICING_2025 
+ 6. Save</t>
+  </si>
+  <si>
+    <t>1. Limit saved with correct pricing 
+ 2. Pricing info reflected in inquiry 
+ 3. Limit visible in unconfirmed list</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7500,6 +7917,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -12482,10 +12904,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB919F80-9B96-4E34-ADD6-E7884B62F830}">
-  <dimension ref="A1:Q101"/>
+  <dimension ref="A1:Q111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="A1:Q101"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="51.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13614,7 +14036,7 @@
         <v>658</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>1089</v>
+        <v>1109</v>
       </c>
       <c r="P21" s="4" t="s">
         <v>754</v>
@@ -13624,10 +14046,10 @@
       </c>
     </row>
     <row r="22" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="6">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>794</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -13677,10 +14099,10 @@
       </c>
     </row>
     <row r="23" spans="1:17" ht="72" x14ac:dyDescent="0.3">
-      <c r="A23" s="6">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>803</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -13730,10 +14152,10 @@
       </c>
     </row>
     <row r="24" spans="1:17" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="6">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>812</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -13783,10 +14205,10 @@
       </c>
     </row>
     <row r="25" spans="1:17" ht="72" x14ac:dyDescent="0.3">
-      <c r="A25" s="6">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>819</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -13836,10 +14258,10 @@
       </c>
     </row>
     <row r="26" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="6">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>826</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -13889,10 +14311,10 @@
       </c>
     </row>
     <row r="27" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="6">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>832</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -13942,10 +14364,10 @@
       </c>
     </row>
     <row r="28" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="6">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>839</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -13995,10 +14417,10 @@
       </c>
     </row>
     <row r="29" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="6">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>846</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -14048,10 +14470,10 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="6">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>853</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -14101,10 +14523,10 @@
       </c>
     </row>
     <row r="31" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="6">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>860</v>
       </c>
       <c r="C31" s="6" t="s">
@@ -14154,10 +14576,10 @@
       </c>
     </row>
     <row r="32" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="6">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>874</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -14207,10 +14629,10 @@
       </c>
     </row>
     <row r="33" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="6">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>881</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -14260,10 +14682,10 @@
       </c>
     </row>
     <row r="34" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="6">
+      <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>887</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -14313,10 +14735,10 @@
       </c>
     </row>
     <row r="35" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="6">
+      <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="4" t="s">
         <v>893</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -14366,10 +14788,10 @@
       </c>
     </row>
     <row r="36" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="6">
+      <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>900</v>
       </c>
       <c r="C36" s="6" t="s">
@@ -14419,10 +14841,10 @@
       </c>
     </row>
     <row r="37" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="6">
+      <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="4" t="s">
         <v>908</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -14472,10 +14894,10 @@
       </c>
     </row>
     <row r="38" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="6">
+      <c r="A38" s="4">
         <v>37</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="4" t="s">
         <v>915</v>
       </c>
       <c r="C38" s="6" t="s">
@@ -14525,10 +14947,10 @@
       </c>
     </row>
     <row r="39" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="6">
+      <c r="A39" s="4">
         <v>38</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="4" t="s">
         <v>922</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -14578,10 +15000,10 @@
       </c>
     </row>
     <row r="40" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="6">
+      <c r="A40" s="4">
         <v>39</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="4" t="s">
         <v>929</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -14631,10 +15053,10 @@
       </c>
     </row>
     <row r="41" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="6">
+      <c r="A41" s="4">
         <v>40</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="4" t="s">
         <v>936</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -14684,10 +15106,10 @@
       </c>
     </row>
     <row r="42" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="6">
+      <c r="A42" s="4">
         <v>41</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>943</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -14737,10 +15159,10 @@
       </c>
     </row>
     <row r="43" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="6">
+      <c r="A43" s="4">
         <v>42</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="4" t="s">
         <v>950</v>
       </c>
       <c r="C43" s="6" t="s">
@@ -14790,10 +15212,10 @@
       </c>
     </row>
     <row r="44" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="6">
+      <c r="A44" s="4">
         <v>43</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="4" t="s">
         <v>957</v>
       </c>
       <c r="C44" s="6" t="s">
@@ -14843,10 +15265,10 @@
       </c>
     </row>
     <row r="45" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="6">
+      <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="4" t="s">
         <v>964</v>
       </c>
       <c r="C45" s="6" t="s">
@@ -14896,10 +15318,10 @@
       </c>
     </row>
     <row r="46" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="6">
+      <c r="A46" s="4">
         <v>45</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="4" t="s">
         <v>971</v>
       </c>
       <c r="C46" s="6" t="s">
@@ -14949,10 +15371,10 @@
       </c>
     </row>
     <row r="47" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A47" s="6">
+      <c r="A47" s="4">
         <v>46</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="4" t="s">
         <v>978</v>
       </c>
       <c r="C47" s="6" t="s">
@@ -15002,10 +15424,10 @@
       </c>
     </row>
     <row r="48" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="6">
+      <c r="A48" s="4">
         <v>47</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="4" t="s">
         <v>985</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -15055,10 +15477,10 @@
       </c>
     </row>
     <row r="49" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="6">
+      <c r="A49" s="4">
         <v>48</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="4" t="s">
         <v>991</v>
       </c>
       <c r="C49" s="6" t="s">
@@ -15098,7 +15520,7 @@
         <v>989</v>
       </c>
       <c r="O49" s="6" t="s">
-        <v>1090</v>
+        <v>1110</v>
       </c>
       <c r="P49" s="6" t="s">
         <v>990</v>
@@ -15108,10 +15530,10 @@
       </c>
     </row>
     <row r="50" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A50" s="6">
+      <c r="A50" s="4">
         <v>49</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="4" t="s">
         <v>998</v>
       </c>
       <c r="C50" s="6" t="s">
@@ -15161,10 +15583,10 @@
       </c>
     </row>
     <row r="51" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="6">
+      <c r="A51" s="4">
         <v>50</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="4" t="s">
         <v>1004</v>
       </c>
       <c r="C51" s="6" t="s">
@@ -15204,7 +15626,7 @@
         <v>1002</v>
       </c>
       <c r="O51" s="6" t="s">
-        <v>1091</v>
+        <v>1111</v>
       </c>
       <c r="P51" s="6" t="s">
         <v>1003</v>
@@ -15214,10 +15636,10 @@
       </c>
     </row>
     <row r="52" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A52" s="6">
+      <c r="A52" s="4">
         <v>51</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="4" t="s">
         <v>1011</v>
       </c>
       <c r="C52" s="6" t="s">
@@ -15267,10 +15689,10 @@
       </c>
     </row>
     <row r="53" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A53" s="6">
+      <c r="A53" s="4">
         <v>52</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="4" t="s">
         <v>1019</v>
       </c>
       <c r="C53" s="6" t="s">
@@ -15320,10 +15742,10 @@
       </c>
     </row>
     <row r="54" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="6">
+      <c r="A54" s="4">
         <v>53</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="4" t="s">
         <v>1026</v>
       </c>
       <c r="C54" s="6" t="s">
@@ -15363,7 +15785,7 @@
         <v>1024</v>
       </c>
       <c r="O54" s="6" t="s">
-        <v>1092</v>
+        <v>1112</v>
       </c>
       <c r="P54" s="6" t="s">
         <v>1025</v>
@@ -15373,10 +15795,10 @@
       </c>
     </row>
     <row r="55" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A55" s="6">
+      <c r="A55" s="4">
         <v>54</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="4" t="s">
         <v>1031</v>
       </c>
       <c r="C55" s="6" t="s">
@@ -15416,7 +15838,7 @@
         <v>658</v>
       </c>
       <c r="O55" s="6" t="s">
-        <v>1093</v>
+        <v>1113</v>
       </c>
       <c r="P55" s="6" t="s">
         <v>1030</v>
@@ -15426,10 +15848,10 @@
       </c>
     </row>
     <row r="56" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A56" s="6">
+      <c r="A56" s="4">
         <v>55</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="4" t="s">
         <v>1035</v>
       </c>
       <c r="C56" s="6" t="s">
@@ -15469,7 +15891,7 @@
         <v>658</v>
       </c>
       <c r="O56" s="6" t="s">
-        <v>1094</v>
+        <v>1114</v>
       </c>
       <c r="P56" s="6" t="s">
         <v>1034</v>
@@ -15479,10 +15901,10 @@
       </c>
     </row>
     <row r="57" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="6">
+      <c r="A57" s="4">
         <v>56</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="4" t="s">
         <v>1042</v>
       </c>
       <c r="C57" s="6" t="s">
@@ -15522,7 +15944,7 @@
         <v>658</v>
       </c>
       <c r="O57" s="6" t="s">
-        <v>1095</v>
+        <v>1115</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>1041</v>
@@ -15532,10 +15954,10 @@
       </c>
     </row>
     <row r="58" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A58" s="6">
+      <c r="A58" s="4">
         <v>57</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="4" t="s">
         <v>1051</v>
       </c>
       <c r="C58" s="6" t="s">
@@ -15585,10 +16007,10 @@
       </c>
     </row>
     <row r="59" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="6">
+      <c r="A59" s="4">
         <v>58</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="4" t="s">
         <v>1057</v>
       </c>
       <c r="C59" s="6" t="s">
@@ -15628,7 +16050,7 @@
         <v>1055</v>
       </c>
       <c r="O59" s="6" t="s">
-        <v>1096</v>
+        <v>1116</v>
       </c>
       <c r="P59" s="6" t="s">
         <v>1056</v>
@@ -15638,11 +16060,11 @@
       </c>
     </row>
     <row r="60" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="6">
+      <c r="A60" s="4">
         <v>59</v>
       </c>
-      <c r="B60" s="6" t="s">
-        <v>1097</v>
+      <c r="B60" s="4" t="s">
+        <v>1117</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>1058</v>
@@ -15681,7 +16103,7 @@
         <v>1061</v>
       </c>
       <c r="O60" s="6" t="s">
-        <v>1098</v>
+        <v>1118</v>
       </c>
       <c r="P60" s="6" t="s">
         <v>1062</v>
@@ -15691,11 +16113,11 @@
       </c>
     </row>
     <row r="61" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="6">
+      <c r="A61" s="4">
         <v>60</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>1099</v>
+      <c r="B61" s="4" t="s">
+        <v>1119</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>1065</v>
@@ -15728,13 +16150,13 @@
         <v>45823</v>
       </c>
       <c r="M61" s="6" t="s">
-        <v>1100</v>
+        <v>1120</v>
       </c>
       <c r="N61" s="6" t="s">
         <v>1068</v>
       </c>
       <c r="O61" s="6" t="s">
-        <v>1101</v>
+        <v>1121</v>
       </c>
       <c r="P61" s="6" t="s">
         <v>1069</v>
@@ -15743,24 +16165,24 @@
         <v>658</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="72" x14ac:dyDescent="0.3">
-      <c r="A62" s="6">
+    <row r="62" spans="1:17" ht="216" x14ac:dyDescent="0.3">
+      <c r="A62" s="4">
         <v>61</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="4" t="s">
         <v>1064</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>1102</v>
+        <v>1122</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>1103</v>
+        <v>1123</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>1104</v>
+        <v>1124</v>
       </c>
       <c r="G62" s="6" t="s">
         <v>654</v>
@@ -15781,33 +16203,33 @@
         <v>45823</v>
       </c>
       <c r="M62" s="6" t="s">
-        <v>1105</v>
+        <v>1286</v>
       </c>
       <c r="N62" s="6" t="s">
-        <v>1106</v>
+        <v>1125</v>
       </c>
       <c r="O62" s="6" t="s">
-        <v>1107</v>
+        <v>1287</v>
       </c>
       <c r="P62" s="6" t="s">
-        <v>1108</v>
+        <v>1126</v>
       </c>
       <c r="Q62" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="6">
+    <row r="63" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="4">
         <v>62</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="4" t="s">
         <v>1070</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>1109</v>
+        <v>1127</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>1110</v>
+        <v>1128</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>3</v>
@@ -15834,39 +16256,39 @@
         <v>45823</v>
       </c>
       <c r="M63" s="6" t="s">
-        <v>1111</v>
+        <v>1288</v>
       </c>
       <c r="N63" s="6" t="s">
-        <v>1112</v>
+        <v>1129</v>
       </c>
       <c r="O63" s="6" t="s">
-        <v>1113</v>
+        <v>1289</v>
       </c>
       <c r="P63" s="6" t="s">
-        <v>1114</v>
+        <v>1130</v>
       </c>
       <c r="Q63" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A64" s="6">
+    <row r="64" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="4">
         <v>63</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="4" t="s">
         <v>1071</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>1115</v>
+        <v>1131</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>1116</v>
+        <v>1132</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>1117</v>
+        <v>1133</v>
       </c>
       <c r="G64" s="6" t="s">
         <v>654</v>
@@ -15887,39 +16309,39 @@
         <v>45823</v>
       </c>
       <c r="M64" s="6" t="s">
-        <v>1118</v>
+        <v>1290</v>
       </c>
       <c r="N64" s="6" t="s">
-        <v>1119</v>
+        <v>1134</v>
       </c>
       <c r="O64" s="6" t="s">
-        <v>1120</v>
+        <v>1291</v>
       </c>
       <c r="P64" s="6" t="s">
-        <v>1121</v>
+        <v>1135</v>
       </c>
       <c r="Q64" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A65" s="6">
+    <row r="65" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="4">
         <v>64</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="4" t="s">
         <v>1072</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>1122</v>
+        <v>1136</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>1123</v>
+        <v>1137</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>1124</v>
+        <v>1138</v>
       </c>
       <c r="G65" s="6" t="s">
         <v>654</v>
@@ -15931,7 +16353,7 @@
         <v>655</v>
       </c>
       <c r="J65" s="6" t="s">
-        <v>1125</v>
+        <v>1139</v>
       </c>
       <c r="K65" s="6" t="s">
         <v>0</v>
@@ -15940,39 +16362,39 @@
         <v>45823</v>
       </c>
       <c r="M65" s="6" t="s">
-        <v>1126</v>
+        <v>1292</v>
       </c>
       <c r="N65" s="6" t="s">
-        <v>1127</v>
+        <v>1140</v>
       </c>
       <c r="O65" s="6" t="s">
-        <v>1128</v>
+        <v>1293</v>
       </c>
       <c r="P65" s="6" t="s">
-        <v>1129</v>
+        <v>1141</v>
       </c>
       <c r="Q65" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A66" s="6">
+    <row r="66" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="4">
         <v>65</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="4" t="s">
         <v>1073</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>1130</v>
+        <v>1142</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>1131</v>
+        <v>1143</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>1132</v>
+        <v>1144</v>
       </c>
       <c r="G66" s="6" t="s">
         <v>654</v>
@@ -15984,7 +16406,7 @@
         <v>655</v>
       </c>
       <c r="J66" s="6" t="s">
-        <v>1125</v>
+        <v>1139</v>
       </c>
       <c r="K66" s="6" t="s">
         <v>0</v>
@@ -15993,39 +16415,39 @@
         <v>45823</v>
       </c>
       <c r="M66" s="6" t="s">
-        <v>1133</v>
+        <v>1294</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>1134</v>
+        <v>1145</v>
       </c>
       <c r="O66" s="6" t="s">
-        <v>1135</v>
+        <v>1295</v>
       </c>
       <c r="P66" s="6" t="s">
-        <v>1136</v>
+        <v>1146</v>
       </c>
       <c r="Q66" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A67" s="6">
+    <row r="67" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="4">
         <v>66</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="4" t="s">
         <v>1074</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>1137</v>
+        <v>1147</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>1138</v>
+        <v>1148</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>1139</v>
+        <v>1149</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>654</v>
@@ -16046,39 +16468,39 @@
         <v>45823</v>
       </c>
       <c r="M67" s="6" t="s">
-        <v>1140</v>
+        <v>1296</v>
       </c>
       <c r="N67" s="6" t="s">
-        <v>1141</v>
+        <v>1150</v>
       </c>
       <c r="O67" s="6" t="s">
-        <v>1142</v>
+        <v>1297</v>
       </c>
       <c r="P67" s="6" t="s">
-        <v>1143</v>
+        <v>1151</v>
       </c>
       <c r="Q67" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="6">
+    <row r="68" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="4">
         <v>67</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="4" t="s">
         <v>1075</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>1144</v>
+        <v>1152</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>1145</v>
+        <v>1153</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>1146</v>
+        <v>1154</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>654</v>
@@ -16099,39 +16521,39 @@
         <v>45823</v>
       </c>
       <c r="M68" s="6" t="s">
-        <v>1147</v>
+        <v>1298</v>
       </c>
       <c r="N68" s="6" t="s">
-        <v>1148</v>
+        <v>1155</v>
       </c>
       <c r="O68" s="6" t="s">
-        <v>1149</v>
+        <v>1299</v>
       </c>
       <c r="P68" s="6" t="s">
-        <v>1150</v>
+        <v>1156</v>
       </c>
       <c r="Q68" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A69" s="6">
+    <row r="69" spans="1:17" ht="144" x14ac:dyDescent="0.3">
+      <c r="A69" s="4">
         <v>68</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="4" t="s">
         <v>1076</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>1151</v>
+        <v>1157</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>1152</v>
+        <v>1158</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>1153</v>
+        <v>1159</v>
       </c>
       <c r="G69" s="6" t="s">
         <v>654</v>
@@ -16143,7 +16565,7 @@
         <v>655</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>1125</v>
+        <v>1139</v>
       </c>
       <c r="K69" s="6" t="s">
         <v>0</v>
@@ -16152,39 +16574,39 @@
         <v>45823</v>
       </c>
       <c r="M69" s="6" t="s">
-        <v>1154</v>
+        <v>1300</v>
       </c>
       <c r="N69" s="6" t="s">
-        <v>1155</v>
+        <v>1160</v>
       </c>
       <c r="O69" s="6" t="s">
-        <v>1156</v>
+        <v>1301</v>
       </c>
       <c r="P69" s="6" t="s">
-        <v>1157</v>
+        <v>1161</v>
       </c>
       <c r="Q69" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="6">
+    <row r="70" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="4">
         <v>69</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="4" t="s">
         <v>1077</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>1158</v>
+        <v>1162</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>1159</v>
+        <v>1163</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>1160</v>
+        <v>1164</v>
       </c>
       <c r="G70" s="6" t="s">
         <v>654</v>
@@ -16196,7 +16618,7 @@
         <v>655</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>1125</v>
+        <v>1139</v>
       </c>
       <c r="K70" s="6" t="s">
         <v>0</v>
@@ -16205,39 +16627,39 @@
         <v>45823</v>
       </c>
       <c r="M70" s="6" t="s">
-        <v>1161</v>
+        <v>1302</v>
       </c>
       <c r="N70" s="6" t="s">
-        <v>1162</v>
+        <v>1165</v>
       </c>
       <c r="O70" s="6" t="s">
-        <v>1163</v>
+        <v>1303</v>
       </c>
       <c r="P70" s="6" t="s">
-        <v>1164</v>
+        <v>1166</v>
       </c>
       <c r="Q70" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A71" s="6">
+    <row r="71" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="4">
         <v>70</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="4" t="s">
         <v>1078</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>1165</v>
+        <v>1167</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>1166</v>
+        <v>1168</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>1167</v>
+        <v>1169</v>
       </c>
       <c r="G71" s="6" t="s">
         <v>654</v>
@@ -16249,7 +16671,7 @@
         <v>655</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>1125</v>
+        <v>1139</v>
       </c>
       <c r="K71" s="6" t="s">
         <v>0</v>
@@ -16258,13 +16680,13 @@
         <v>45823</v>
       </c>
       <c r="M71" s="6" t="s">
-        <v>1168</v>
+        <v>1304</v>
       </c>
       <c r="N71" s="6" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="O71" s="6" t="s">
-        <v>1170</v>
+        <v>1305</v>
       </c>
       <c r="P71" s="6" t="s">
         <v>1171</v>
@@ -16273,11 +16695,11 @@
         <v>658</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A72" s="6">
+    <row r="72" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="4">
         <v>71</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="4" t="s">
         <v>1079</v>
       </c>
       <c r="C72" s="6" t="s">
@@ -16311,39 +16733,39 @@
         <v>45823</v>
       </c>
       <c r="M72" s="6" t="s">
+        <v>1306</v>
+      </c>
+      <c r="N72" s="6" t="s">
         <v>1175</v>
       </c>
-      <c r="N72" s="6" t="s">
+      <c r="O72" s="6" t="s">
+        <v>1307</v>
+      </c>
+      <c r="P72" s="6" t="s">
         <v>1176</v>
-      </c>
-      <c r="O72" s="6" t="s">
-        <v>1177</v>
-      </c>
-      <c r="P72" s="6" t="s">
-        <v>1178</v>
       </c>
       <c r="Q72" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A73" s="6">
+    <row r="73" spans="1:17" ht="144" x14ac:dyDescent="0.3">
+      <c r="A73" s="4">
         <v>72</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="4" t="s">
         <v>1080</v>
       </c>
       <c r="C73" s="6" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F73" s="6" t="s">
         <v>1179</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>1180</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>1181</v>
       </c>
       <c r="G73" s="6" t="s">
         <v>654</v>
@@ -16364,39 +16786,39 @@
         <v>45823</v>
       </c>
       <c r="M73" s="6" t="s">
-        <v>1182</v>
+        <v>1308</v>
       </c>
       <c r="N73" s="6" t="s">
-        <v>1183</v>
+        <v>1180</v>
       </c>
       <c r="O73" s="6" t="s">
-        <v>1184</v>
+        <v>1309</v>
       </c>
       <c r="P73" s="6" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="Q73" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="6">
+    <row r="74" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="4">
         <v>73</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B74" s="4" t="s">
         <v>1081</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="G74" s="6" t="s">
         <v>654</v>
@@ -16408,7 +16830,7 @@
         <v>655</v>
       </c>
       <c r="J74" s="6" t="s">
-        <v>1125</v>
+        <v>1139</v>
       </c>
       <c r="K74" s="6" t="s">
         <v>0</v>
@@ -16417,39 +16839,39 @@
         <v>45823</v>
       </c>
       <c r="M74" s="6" t="s">
-        <v>1189</v>
+        <v>1310</v>
       </c>
       <c r="N74" s="6" t="s">
-        <v>1190</v>
+        <v>1185</v>
       </c>
       <c r="O74" s="6" t="s">
-        <v>1191</v>
+        <v>1311</v>
       </c>
       <c r="P74" s="6" t="s">
-        <v>1192</v>
+        <v>1186</v>
       </c>
       <c r="Q74" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="75" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="6">
+    <row r="75" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="4">
         <v>74</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="4" t="s">
         <v>1082</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>1193</v>
+        <v>1187</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>1194</v>
+        <v>1188</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>1195</v>
+        <v>1189</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>654</v>
@@ -16461,7 +16883,7 @@
         <v>655</v>
       </c>
       <c r="J75" s="6" t="s">
-        <v>1125</v>
+        <v>1139</v>
       </c>
       <c r="K75" s="6" t="s">
         <v>0</v>
@@ -16470,39 +16892,39 @@
         <v>45823</v>
       </c>
       <c r="M75" s="6" t="s">
-        <v>1196</v>
+        <v>1312</v>
       </c>
       <c r="N75" s="6" t="s">
-        <v>1197</v>
+        <v>1190</v>
       </c>
       <c r="O75" s="6" t="s">
-        <v>1198</v>
+        <v>1313</v>
       </c>
       <c r="P75" s="6" t="s">
-        <v>1199</v>
+        <v>1191</v>
       </c>
       <c r="Q75" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="76" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="6">
+    <row r="76" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="4">
         <v>75</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="B76" s="4" t="s">
         <v>1083</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>1200</v>
+        <v>1192</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>1201</v>
+        <v>1193</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>1202</v>
+        <v>1194</v>
       </c>
       <c r="G76" s="6" t="s">
         <v>654</v>
@@ -16514,7 +16936,7 @@
         <v>655</v>
       </c>
       <c r="J76" s="6" t="s">
-        <v>1125</v>
+        <v>1139</v>
       </c>
       <c r="K76" s="6" t="s">
         <v>0</v>
@@ -16523,39 +16945,39 @@
         <v>45823</v>
       </c>
       <c r="M76" s="6" t="s">
-        <v>1203</v>
+        <v>1314</v>
       </c>
       <c r="N76" s="6" t="s">
-        <v>1204</v>
+        <v>1195</v>
       </c>
       <c r="O76" s="6" t="s">
-        <v>1205</v>
+        <v>1315</v>
       </c>
       <c r="P76" s="6" t="s">
-        <v>1206</v>
+        <v>1196</v>
       </c>
       <c r="Q76" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A77" s="6">
+    <row r="77" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="4">
         <v>76</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="4" t="s">
         <v>1084</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>1130</v>
+        <v>1142</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>1207</v>
+        <v>1197</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>1208</v>
+        <v>1198</v>
       </c>
       <c r="G77" s="6" t="s">
         <v>654</v>
@@ -16567,7 +16989,7 @@
         <v>655</v>
       </c>
       <c r="J77" s="6" t="s">
-        <v>1125</v>
+        <v>1139</v>
       </c>
       <c r="K77" s="6" t="s">
         <v>0</v>
@@ -16576,39 +16998,39 @@
         <v>45823</v>
       </c>
       <c r="M77" s="6" t="s">
-        <v>1209</v>
+        <v>1316</v>
       </c>
       <c r="N77" s="6" t="s">
-        <v>1210</v>
+        <v>1199</v>
       </c>
       <c r="O77" s="6" t="s">
-        <v>1211</v>
+        <v>1317</v>
       </c>
       <c r="P77" s="6" t="s">
-        <v>1212</v>
+        <v>1200</v>
       </c>
       <c r="Q77" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A78" s="6">
+    <row r="78" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="4">
         <v>77</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="4" t="s">
         <v>1085</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>1213</v>
+        <v>1201</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>1214</v>
+        <v>1202</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>1215</v>
+        <v>1203</v>
       </c>
       <c r="G78" s="6" t="s">
         <v>654</v>
@@ -16629,39 +17051,39 @@
         <v>45823</v>
       </c>
       <c r="M78" s="6" t="s">
-        <v>1216</v>
+        <v>1318</v>
       </c>
       <c r="N78" s="6" t="s">
-        <v>1217</v>
+        <v>1204</v>
       </c>
       <c r="O78" s="6" t="s">
-        <v>1218</v>
+        <v>1319</v>
       </c>
       <c r="P78" s="6" t="s">
-        <v>1219</v>
+        <v>1205</v>
       </c>
       <c r="Q78" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A79" s="6">
+    <row r="79" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="4">
         <v>78</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="4" t="s">
         <v>1086</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>1220</v>
+        <v>1206</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>1221</v>
+        <v>1207</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>1222</v>
+        <v>1208</v>
       </c>
       <c r="G79" s="6" t="s">
         <v>654</v>
@@ -16682,39 +17104,39 @@
         <v>45823</v>
       </c>
       <c r="M79" s="6" t="s">
-        <v>1223</v>
+        <v>1320</v>
       </c>
       <c r="N79" s="6" t="s">
-        <v>1224</v>
+        <v>1209</v>
       </c>
       <c r="O79" s="6" t="s">
-        <v>1225</v>
+        <v>1321</v>
       </c>
       <c r="P79" s="6" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="Q79" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A80" s="6">
+    <row r="80" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="4">
         <v>79</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B80" s="4" t="s">
         <v>1087</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>1228</v>
+        <v>1212</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>1229</v>
+        <v>1213</v>
       </c>
       <c r="G80" s="6" t="s">
         <v>654</v>
@@ -16726,7 +17148,7 @@
         <v>655</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>1125</v>
+        <v>1139</v>
       </c>
       <c r="K80" s="6" t="s">
         <v>0</v>
@@ -16735,39 +17157,39 @@
         <v>45823</v>
       </c>
       <c r="M80" s="6" t="s">
-        <v>1230</v>
+        <v>1322</v>
       </c>
       <c r="N80" s="6" t="s">
-        <v>1231</v>
+        <v>1214</v>
       </c>
       <c r="O80" s="6" t="s">
-        <v>1232</v>
+        <v>1323</v>
       </c>
       <c r="P80" s="6" t="s">
-        <v>1233</v>
+        <v>1215</v>
       </c>
       <c r="Q80" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="81" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A81" s="6">
+    <row r="81" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="4">
         <v>80</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="B81" s="4" t="s">
         <v>1088</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>1234</v>
+        <v>1216</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>1235</v>
+        <v>1217</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>1236</v>
+        <v>1218</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>654</v>
@@ -16779,7 +17201,7 @@
         <v>655</v>
       </c>
       <c r="J81" s="6" t="s">
-        <v>1125</v>
+        <v>1139</v>
       </c>
       <c r="K81" s="6" t="s">
         <v>0</v>
@@ -16788,1019 +17210,1050 @@
         <v>45823</v>
       </c>
       <c r="M81" s="6" t="s">
-        <v>1237</v>
+        <v>1324</v>
       </c>
       <c r="N81" s="6" t="s">
-        <v>1238</v>
+        <v>1219</v>
       </c>
       <c r="O81" s="6" t="s">
-        <v>1239</v>
+        <v>1325</v>
       </c>
       <c r="P81" s="6" t="s">
-        <v>1240</v>
+        <v>1220</v>
       </c>
       <c r="Q81" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="82" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A82" s="6">
+    <row r="82" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A82" s="4">
         <v>81</v>
       </c>
-      <c r="B82" s="6" t="s">
-        <v>232</v>
+      <c r="B82" s="4" t="s">
+        <v>1089</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>1241</v>
+        <v>1221</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>1242</v>
+        <v>1326</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>1243</v>
+        <v>1222</v>
       </c>
       <c r="G82" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I82" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J82" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K82" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L82" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M82" s="6" t="s">
-        <v>1248</v>
+        <v>1327</v>
       </c>
       <c r="N82" s="6" t="s">
-        <v>1249</v>
+        <v>1227</v>
       </c>
       <c r="O82" s="6" t="s">
-        <v>1250</v>
+        <v>1328</v>
       </c>
       <c r="P82" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A83" s="6">
+    <row r="83" spans="1:17" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A83" s="4">
         <v>82</v>
       </c>
-      <c r="B83" s="6" t="s">
-        <v>234</v>
+      <c r="B83" s="4" t="s">
+        <v>1090</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>1251</v>
+        <v>1228</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>1252</v>
+        <v>1329</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>1253</v>
+        <v>1229</v>
       </c>
       <c r="G83" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H83" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I83" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J83" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K83" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L83" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M83" s="6" t="s">
-        <v>1254</v>
+        <v>1330</v>
       </c>
       <c r="N83" s="6" t="s">
-        <v>1255</v>
+        <v>1230</v>
       </c>
       <c r="O83" s="6" t="s">
-        <v>1256</v>
+        <v>1331</v>
       </c>
       <c r="P83" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:17" ht="72" x14ac:dyDescent="0.3">
-      <c r="A84" s="6">
+    <row r="84" spans="1:17" ht="216" x14ac:dyDescent="0.3">
+      <c r="A84" s="4">
         <v>83</v>
       </c>
-      <c r="B84" s="6" t="s">
-        <v>237</v>
+      <c r="B84" s="4" t="s">
+        <v>1091</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>1257</v>
+        <v>1231</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>1258</v>
+        <v>1332</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>1259</v>
+        <v>1232</v>
       </c>
       <c r="G84" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H84" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I84" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J84" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K84" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L84" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M84" s="6" t="s">
-        <v>1260</v>
+        <v>1333</v>
       </c>
       <c r="N84" s="6" t="s">
-        <v>1261</v>
+        <v>1233</v>
       </c>
       <c r="O84" s="6" t="s">
-        <v>1262</v>
+        <v>1334</v>
       </c>
       <c r="P84" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:17" ht="72" x14ac:dyDescent="0.3">
-      <c r="A85" s="6">
+    <row r="85" spans="1:17" ht="216" x14ac:dyDescent="0.3">
+      <c r="A85" s="4">
         <v>84</v>
       </c>
-      <c r="B85" s="6" t="s">
-        <v>240</v>
+      <c r="B85" s="4" t="s">
+        <v>1092</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>1263</v>
+        <v>1234</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>1264</v>
+        <v>1335</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>1265</v>
+        <v>1235</v>
       </c>
       <c r="G85" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I85" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J85" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L85" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M85" s="6" t="s">
-        <v>1266</v>
+        <v>1336</v>
       </c>
       <c r="N85" s="6" t="s">
-        <v>1267</v>
+        <v>1337</v>
       </c>
       <c r="O85" s="6" t="s">
-        <v>1268</v>
+        <v>1338</v>
       </c>
       <c r="P85" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A86" s="6">
+    <row r="86" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A86" s="4">
         <v>85</v>
       </c>
-      <c r="B86" s="6" t="s">
-        <v>243</v>
+      <c r="B86" s="4" t="s">
+        <v>1093</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>1269</v>
+        <v>1236</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>1270</v>
+        <v>1237</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>1271</v>
+        <v>1238</v>
       </c>
       <c r="G86" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H86" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I86" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J86" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K86" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L86" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M86" s="6" t="s">
-        <v>1272</v>
+        <v>1339</v>
       </c>
       <c r="N86" s="6" t="s">
-        <v>1273</v>
+        <v>1239</v>
       </c>
       <c r="O86" s="6" t="s">
-        <v>1274</v>
+        <v>1340</v>
       </c>
       <c r="P86" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A87" s="6">
+    <row r="87" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A87" s="4">
         <v>86</v>
       </c>
-      <c r="B87" s="6" t="s">
-        <v>245</v>
+      <c r="B87" s="4" t="s">
+        <v>1094</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>1275</v>
+        <v>1240</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>1276</v>
+        <v>1241</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>1277</v>
+        <v>1242</v>
       </c>
       <c r="G87" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H87" s="6" t="s">
+        <v>1223</v>
+      </c>
+      <c r="I87" s="6" t="s">
+        <v>1224</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K87" s="6" t="s">
+        <v>1225</v>
+      </c>
+      <c r="L87" s="7" t="s">
+        <v>1226</v>
+      </c>
+      <c r="M87" s="6" t="s">
+        <v>1341</v>
+      </c>
+      <c r="N87" s="6" t="s">
+        <v>1243</v>
+      </c>
+      <c r="O87" s="6" t="s">
+        <v>1342</v>
+      </c>
+      <c r="P87" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="4">
+        <v>87</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C88" s="6" t="s">
         <v>1244</v>
       </c>
-      <c r="I87" s="6" t="s">
+      <c r="D88" s="6" t="s">
+        <v>1343</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F88" s="6" t="s">
         <v>1245</v>
-      </c>
-      <c r="J87" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="K87" s="6" t="s">
-        <v>1246</v>
-      </c>
-      <c r="L87" s="7" t="s">
-        <v>1247</v>
-      </c>
-      <c r="M87" s="6" t="s">
-        <v>1278</v>
-      </c>
-      <c r="N87" s="6" t="s">
-        <v>1279</v>
-      </c>
-      <c r="O87" s="6" t="s">
-        <v>1280</v>
-      </c>
-      <c r="P87" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="6">
-        <v>87</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>1281</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>1282</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F88" s="6" t="s">
-        <v>1283</v>
       </c>
       <c r="G88" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I88" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J88" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K88" s="6" t="s">
+        <v>1225</v>
+      </c>
+      <c r="L88" s="7" t="s">
+        <v>1226</v>
+      </c>
+      <c r="M88" s="6" t="s">
+        <v>1344</v>
+      </c>
+      <c r="N88" s="6" t="s">
         <v>1246</v>
       </c>
-      <c r="L88" s="7" t="s">
+      <c r="O88" s="6" t="s">
+        <v>1345</v>
+      </c>
+      <c r="P88" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A89" s="4">
+        <v>88</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C89" s="6" t="s">
         <v>1247</v>
       </c>
-      <c r="M88" s="6" t="s">
-        <v>1284</v>
-      </c>
-      <c r="N88" s="6" t="s">
-        <v>1285</v>
-      </c>
-      <c r="O88" s="6" t="s">
-        <v>1286</v>
-      </c>
-      <c r="P88" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A89" s="6">
-        <v>88</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>1287</v>
-      </c>
       <c r="D89" s="6" t="s">
-        <v>1288</v>
+        <v>1346</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>1289</v>
+        <v>1248</v>
       </c>
       <c r="G89" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H89" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I89" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J89" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L89" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M89" s="6" t="s">
-        <v>1290</v>
+        <v>1347</v>
       </c>
       <c r="N89" s="6" t="s">
-        <v>1291</v>
+        <v>1249</v>
       </c>
       <c r="O89" s="6" t="s">
-        <v>1292</v>
+        <v>1348</v>
       </c>
       <c r="P89" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A90" s="6">
+    <row r="90" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A90" s="4">
         <v>89</v>
       </c>
-      <c r="B90" s="6" t="s">
-        <v>253</v>
+      <c r="B90" s="4" t="s">
+        <v>1097</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>1293</v>
+        <v>1250</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>1294</v>
+        <v>1251</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>1295</v>
+        <v>1252</v>
       </c>
       <c r="G90" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H90" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I90" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J90" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K90" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L90" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M90" s="6" t="s">
-        <v>1296</v>
+        <v>1349</v>
       </c>
       <c r="N90" s="6" t="s">
-        <v>1297</v>
+        <v>1253</v>
       </c>
       <c r="O90" s="6" t="s">
-        <v>1298</v>
+        <v>1350</v>
       </c>
       <c r="P90" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A91" s="6">
+    <row r="91" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A91" s="4">
         <v>90</v>
       </c>
-      <c r="B91" s="6" t="s">
-        <v>255</v>
+      <c r="B91" s="4" t="s">
+        <v>1098</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>1299</v>
+        <v>1254</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>1300</v>
+        <v>1351</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>1301</v>
+        <v>1255</v>
       </c>
       <c r="G91" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I91" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J91" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K91" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L91" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M91" s="6" t="s">
-        <v>1302</v>
+        <v>1352</v>
       </c>
       <c r="N91" s="6" t="s">
-        <v>1303</v>
+        <v>1256</v>
       </c>
       <c r="O91" s="6" t="s">
-        <v>1304</v>
+        <v>1353</v>
       </c>
       <c r="P91" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="6">
-        <v>11</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>258</v>
+    <row r="92" spans="1:17" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A92" s="4">
+        <v>91</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>1099</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>1305</v>
+        <v>1257</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>1306</v>
+        <v>1354</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>1307</v>
+        <v>1258</v>
       </c>
       <c r="G92" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H92" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I92" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J92" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K92" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L92" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M92" s="6" t="s">
-        <v>1308</v>
+        <v>1355</v>
       </c>
       <c r="N92" s="6" t="s">
-        <v>1309</v>
+        <v>1259</v>
       </c>
       <c r="O92" s="6" t="s">
-        <v>1310</v>
+        <v>1356</v>
       </c>
       <c r="P92" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="6">
-        <v>12</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>261</v>
+    <row r="93" spans="1:17" ht="216" x14ac:dyDescent="0.3">
+      <c r="A93" s="4">
+        <v>92</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>1100</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>1311</v>
+        <v>1260</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>1312</v>
+        <v>1357</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>1313</v>
+        <v>1261</v>
       </c>
       <c r="G93" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I93" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J93" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K93" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L93" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M93" s="6" t="s">
-        <v>1314</v>
+        <v>1358</v>
       </c>
       <c r="N93" s="6" t="s">
-        <v>1315</v>
+        <v>1262</v>
       </c>
       <c r="O93" s="6" t="s">
-        <v>1316</v>
+        <v>1359</v>
       </c>
       <c r="P93" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A94" s="6">
-        <v>13</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>263</v>
+    <row r="94" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A94" s="4">
+        <v>93</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>1101</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>1317</v>
+        <v>1263</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>1318</v>
+        <v>1264</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>1319</v>
+        <v>1265</v>
       </c>
       <c r="G94" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H94" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I94" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J94" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K94" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L94" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M94" s="6" t="s">
-        <v>1320</v>
+        <v>1360</v>
       </c>
       <c r="N94" s="6" t="s">
-        <v>1321</v>
+        <v>1266</v>
       </c>
       <c r="O94" s="6" t="s">
-        <v>1322</v>
+        <v>1361</v>
       </c>
       <c r="P94" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="6">
-        <v>14</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>266</v>
+    <row r="95" spans="1:17" ht="216" x14ac:dyDescent="0.3">
+      <c r="A95" s="4">
+        <v>94</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>1102</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>1323</v>
+        <v>1267</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>1324</v>
+        <v>1362</v>
       </c>
       <c r="E95" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>1325</v>
+        <v>1268</v>
       </c>
       <c r="G95" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H95" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I95" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J95" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K95" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L95" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M95" s="6" t="s">
-        <v>1326</v>
+        <v>1363</v>
       </c>
       <c r="N95" s="6" t="s">
-        <v>1327</v>
+        <v>1269</v>
       </c>
       <c r="O95" s="6" t="s">
-        <v>1328</v>
+        <v>1364</v>
       </c>
       <c r="P95" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A96" s="6">
-        <v>15</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>269</v>
+    <row r="96" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A96" s="4">
+        <v>95</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>1103</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>1329</v>
+        <v>1270</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>1330</v>
+        <v>1365</v>
       </c>
       <c r="E96" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>1331</v>
+        <v>1271</v>
       </c>
       <c r="G96" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I96" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J96" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K96" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L96" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M96" s="6" t="s">
-        <v>1332</v>
+        <v>1366</v>
       </c>
       <c r="N96" s="6" t="s">
-        <v>1333</v>
+        <v>1272</v>
       </c>
       <c r="O96" s="6" t="s">
-        <v>1334</v>
+        <v>1367</v>
       </c>
       <c r="P96" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A97" s="6">
-        <v>16</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>272</v>
+    <row r="97" spans="1:16" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A97" s="4">
+        <v>96</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>1104</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>1335</v>
+        <v>1273</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>1336</v>
+        <v>1368</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>1337</v>
+        <v>1274</v>
       </c>
       <c r="G97" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H97" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I97" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J97" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K97" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L97" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M97" s="6" t="s">
-        <v>1338</v>
+        <v>1369</v>
       </c>
       <c r="N97" s="6" t="s">
-        <v>1339</v>
+        <v>1370</v>
       </c>
       <c r="O97" s="6" t="s">
-        <v>1340</v>
+        <v>1371</v>
       </c>
       <c r="P97" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="144" x14ac:dyDescent="0.3">
-      <c r="A98" s="6">
-        <v>17</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>275</v>
+    <row r="98" spans="1:16" ht="216" x14ac:dyDescent="0.3">
+      <c r="A98" s="4">
+        <v>97</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>1105</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>1341</v>
+        <v>1372</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>1342</v>
+        <v>1275</v>
       </c>
       <c r="F98" s="6" t="s">
         <v>654</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="I98" s="6" t="s">
         <v>0</v>
       </c>
       <c r="J98" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="K98" s="6" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="L98" s="7" t="s">
-        <v>1343</v>
+        <v>1373</v>
       </c>
       <c r="M98" s="6" t="s">
-        <v>1344</v>
+        <v>1276</v>
       </c>
       <c r="N98" s="6" t="s">
-        <v>1345</v>
+        <v>1374</v>
       </c>
       <c r="O98" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A99" s="6">
-        <v>18</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>278</v>
+    <row r="99" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A99" s="4">
+        <v>98</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>1106</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>1346</v>
+        <v>1277</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>1347</v>
+        <v>1375</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F99" s="6" t="s">
-        <v>1348</v>
+        <v>1278</v>
       </c>
       <c r="G99" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H99" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I99" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J99" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K99" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L99" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M99" s="6" t="s">
-        <v>1349</v>
+        <v>1376</v>
       </c>
       <c r="N99" s="6" t="s">
-        <v>1350</v>
+        <v>1279</v>
       </c>
       <c r="O99" s="6" t="s">
-        <v>1351</v>
+        <v>1377</v>
       </c>
       <c r="P99" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A100" s="6">
-        <v>19</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>281</v>
+    <row r="100" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A100" s="4">
+        <v>99</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>1107</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>1352</v>
+        <v>1280</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>1353</v>
+        <v>1281</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>1354</v>
+        <v>1282</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I100" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J100" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K100" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L100" s="7" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M100" s="6" t="s">
-        <v>1355</v>
+        <v>1378</v>
       </c>
       <c r="N100" s="6" t="s">
-        <v>1356</v>
+        <v>1379</v>
       </c>
       <c r="O100" s="6" t="s">
-        <v>1357</v>
+        <v>1380</v>
       </c>
       <c r="P100" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A101" s="6">
-        <v>20</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>284</v>
+    <row r="101" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A101" s="4">
+        <v>100</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>1108</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>1358</v>
+        <v>1283</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>1359</v>
+        <v>1381</v>
       </c>
       <c r="E101" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>1360</v>
+        <v>1284</v>
       </c>
       <c r="G101" s="6" t="s">
         <v>654</v>
       </c>
       <c r="H101" s="6" t="s">
-        <v>1244</v>
+        <v>1223</v>
       </c>
       <c r="I101" s="6" t="s">
-        <v>1245</v>
+        <v>1224</v>
       </c>
       <c r="J101" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K101" s="6" t="s">
-        <v>1246</v>
+        <v>1225</v>
       </c>
       <c r="L101" s="6" t="s">
-        <v>1247</v>
+        <v>1226</v>
       </c>
       <c r="M101" s="6" t="s">
-        <v>1361</v>
+        <v>1382</v>
       </c>
       <c r="N101" s="6" t="s">
-        <v>1362</v>
+        <v>1285</v>
       </c>
       <c r="O101" s="6" t="s">
-        <v>1363</v>
+        <v>1383</v>
       </c>
       <c r="P101" s="6" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B102" s="4"/>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B103" s="4"/>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B104" s="4"/>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B105" s="4"/>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B106" s="4"/>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B107" s="4"/>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B108" s="4"/>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B109" s="4"/>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B110" s="4"/>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B111" s="4"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>